<commit_message>
03/06/2021 covid analisys repot on class
</commit_message>
<xml_diff>
--- a/RMD/output_xlsx/metadata_conf.xlsx
+++ b/RMD/output_xlsx/metadata_conf.xlsx
@@ -1187,7 +1187,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -6232,13 +6232,13 @@
         <v>-100</v>
       </c>
       <c r="D253" t="n">
-        <v>12199764.3042596</v>
+        <v>12199764.8377282</v>
       </c>
       <c r="E253" t="n">
-        <v>12199764.3042596</v>
+        <v>12199764.8377282</v>
       </c>
       <c r="F253" t="n">
-        <v>6014483802</v>
+        <v>6014484065</v>
       </c>
     </row>
     <row r="254">

</xml_diff>

<commit_message>
Final version of Covid19 Notebook
</commit_message>
<xml_diff>
--- a/RMD/output_xlsx/metadata_conf.xlsx
+++ b/RMD/output_xlsx/metadata_conf.xlsx
@@ -1220,13 +1220,13 @@
         <v>67.709953</v>
       </c>
       <c r="D2" t="n">
-        <v>34771.1726907631</v>
+        <v>34852.0300601202</v>
       </c>
       <c r="E2" t="n">
-        <v>34771.1726907631</v>
+        <v>34852.0300601202</v>
       </c>
       <c r="F2" t="n">
-        <v>17316044</v>
+        <v>17391163</v>
       </c>
     </row>
     <row r="3">
@@ -1240,13 +1240,13 @@
         <v>20.1683</v>
       </c>
       <c r="D3" t="n">
-        <v>40759.3995983936</v>
+        <v>40942.9679358717</v>
       </c>
       <c r="E3" t="n">
-        <v>40759.3995983936</v>
+        <v>40942.9679358717</v>
       </c>
       <c r="F3" t="n">
-        <v>20298181</v>
+        <v>20430541</v>
       </c>
     </row>
     <row r="4">
@@ -1260,13 +1260,13 @@
         <v>1.6596</v>
       </c>
       <c r="D4" t="n">
-        <v>56628.2208835341</v>
+        <v>56775.2104208417</v>
       </c>
       <c r="E4" t="n">
-        <v>56628.2208835341</v>
+        <v>56775.2104208417</v>
       </c>
       <c r="F4" t="n">
-        <v>28200854</v>
+        <v>28330830</v>
       </c>
     </row>
     <row r="5">
@@ -1280,13 +1280,13 @@
         <v>1.5218</v>
       </c>
       <c r="D5" t="n">
-        <v>4888.94578313253</v>
+        <v>4906.70741482966</v>
       </c>
       <c r="E5" t="n">
-        <v>4888.94578313253</v>
+        <v>4906.70741482966</v>
       </c>
       <c r="F5" t="n">
-        <v>2434695</v>
+        <v>2448447</v>
       </c>
     </row>
     <row r="6">
@@ -1300,13 +1300,13 @@
         <v>17.8739</v>
       </c>
       <c r="D6" t="n">
-        <v>9846.36947791165</v>
+        <v>9897.05811623247</v>
       </c>
       <c r="E6" t="n">
-        <v>9846.36947791165</v>
+        <v>9897.05811623247</v>
       </c>
       <c r="F6" t="n">
-        <v>4903492</v>
+        <v>4938632</v>
       </c>
     </row>
     <row r="7">
@@ -1320,13 +1320,13 @@
         <v>-61.7964</v>
       </c>
       <c r="D7" t="n">
-        <v>299.0140562249</v>
+        <v>300.943887775551</v>
       </c>
       <c r="E7" t="n">
-        <v>299.0140562249</v>
+        <v>300.943887775551</v>
       </c>
       <c r="F7" t="n">
-        <v>148909</v>
+        <v>150171</v>
       </c>
     </row>
     <row r="8">
@@ -1340,13 +1340,13 @@
         <v>-63.6167</v>
       </c>
       <c r="D8" t="n">
-        <v>1044191.97389558</v>
+        <v>1049883.86773547</v>
       </c>
       <c r="E8" t="n">
-        <v>1044191.97389558</v>
+        <v>1049883.86773547</v>
       </c>
       <c r="F8" t="n">
-        <v>520007603</v>
+        <v>523892050</v>
       </c>
     </row>
     <row r="9">
@@ -1360,13 +1360,13 @@
         <v>45.0382</v>
       </c>
       <c r="D9" t="n">
-        <v>87203.2751004016</v>
+        <v>87475.368737475</v>
       </c>
       <c r="E9" t="n">
-        <v>87203.2751004016</v>
+        <v>87475.368737475</v>
       </c>
       <c r="F9" t="n">
-        <v>43427231</v>
+        <v>43650209</v>
       </c>
     </row>
     <row r="10">
@@ -1380,13 +1380,13 @@
         <v>149.0124</v>
       </c>
       <c r="D10" t="n">
-        <v>99.7068273092369</v>
+        <v>99.7555110220441</v>
       </c>
       <c r="E10" t="n">
-        <v>99.7068273092369</v>
+        <v>99.7555110220441</v>
       </c>
       <c r="F10" t="n">
-        <v>49654</v>
+        <v>49778</v>
       </c>
     </row>
     <row r="11">
@@ -1400,13 +1400,13 @@
         <v>151.2093</v>
       </c>
       <c r="D11" t="n">
-        <v>3754.70682730924</v>
+        <v>3758.38476953908</v>
       </c>
       <c r="E11" t="n">
-        <v>3754.70682730924</v>
+        <v>3758.38476953908</v>
       </c>
       <c r="F11" t="n">
-        <v>1869844</v>
+        <v>1875434</v>
       </c>
     </row>
     <row r="12">
@@ -1420,13 +1420,13 @@
         <v>130.8456</v>
       </c>
       <c r="D12" t="n">
-        <v>57.4277108433735</v>
+        <v>57.6593186372746</v>
       </c>
       <c r="E12" t="n">
-        <v>57.4277108433735</v>
+        <v>57.6593186372746</v>
       </c>
       <c r="F12" t="n">
-        <v>28599</v>
+        <v>28772</v>
       </c>
     </row>
     <row r="13">
@@ -1440,13 +1440,13 @@
         <v>153.0251</v>
       </c>
       <c r="D13" t="n">
-        <v>1064.25100401606</v>
+        <v>1065.36673346693</v>
       </c>
       <c r="E13" t="n">
-        <v>1064.25100401606</v>
+        <v>1065.36673346693</v>
       </c>
       <c r="F13" t="n">
-        <v>529997</v>
+        <v>531618</v>
       </c>
     </row>
     <row r="14">
@@ -1460,13 +1460,13 @@
         <v>138.6007</v>
       </c>
       <c r="D14" t="n">
-        <v>467.638554216867</v>
+        <v>468.224448897796</v>
       </c>
       <c r="E14" t="n">
-        <v>467.638554216867</v>
+        <v>468.224448897796</v>
       </c>
       <c r="F14" t="n">
-        <v>232884</v>
+        <v>233644</v>
       </c>
     </row>
     <row r="15">
@@ -1480,13 +1480,13 @@
         <v>147.3272</v>
       </c>
       <c r="D15" t="n">
-        <v>195.293172690763</v>
+        <v>195.370741482966</v>
       </c>
       <c r="E15" t="n">
-        <v>195.293172690763</v>
+        <v>195.370741482966</v>
       </c>
       <c r="F15" t="n">
-        <v>97256</v>
+        <v>97490</v>
       </c>
     </row>
     <row r="16">
@@ -1500,13 +1500,13 @@
         <v>144.9631</v>
       </c>
       <c r="D16" t="n">
-        <v>12912.3313253012</v>
+        <v>12927.7795591182</v>
       </c>
       <c r="E16" t="n">
-        <v>12912.3313253012</v>
+        <v>12927.7795591182</v>
       </c>
       <c r="F16" t="n">
-        <v>6430341</v>
+        <v>6450962</v>
       </c>
     </row>
     <row r="17">
@@ -1520,13 +1520,13 @@
         <v>115.8605</v>
       </c>
       <c r="D17" t="n">
-        <v>662.066265060241</v>
+        <v>662.779559118236</v>
       </c>
       <c r="E17" t="n">
-        <v>662.066265060241</v>
+        <v>662.779559118236</v>
       </c>
       <c r="F17" t="n">
-        <v>329709</v>
+        <v>330727</v>
       </c>
     </row>
     <row r="18">
@@ -1540,13 +1540,13 @@
         <v>14.5501</v>
       </c>
       <c r="D18" t="n">
-        <v>201899.562248996</v>
+        <v>202789.210420842</v>
       </c>
       <c r="E18" t="n">
-        <v>201899.562248996</v>
+        <v>202789.210420842</v>
       </c>
       <c r="F18" t="n">
-        <v>100545982</v>
+        <v>101191816</v>
       </c>
     </row>
     <row r="19">
@@ -1560,13 +1560,13 @@
         <v>47.5769</v>
       </c>
       <c r="D19" t="n">
-        <v>107837.383534137</v>
+        <v>108291.448897796</v>
       </c>
       <c r="E19" t="n">
-        <v>107837.383534137</v>
+        <v>108291.448897796</v>
       </c>
       <c r="F19" t="n">
-        <v>53703017</v>
+        <v>54037433</v>
       </c>
     </row>
     <row r="20">
@@ -1580,13 +1580,13 @@
         <v>-78.035889</v>
       </c>
       <c r="D20" t="n">
-        <v>4391.80722891566</v>
+        <v>4406.91382765531</v>
       </c>
       <c r="E20" t="n">
-        <v>4391.80722891566</v>
+        <v>4406.91382765531</v>
       </c>
       <c r="F20" t="n">
-        <v>2187120</v>
+        <v>2199050</v>
       </c>
     </row>
     <row r="21">
@@ -1600,13 +1600,13 @@
         <v>50.55</v>
       </c>
       <c r="D21" t="n">
-        <v>70082.2429718876</v>
+        <v>70436.1022044088</v>
       </c>
       <c r="E21" t="n">
-        <v>70082.2429718876</v>
+        <v>70436.1022044088</v>
       </c>
       <c r="F21" t="n">
-        <v>34900957</v>
+        <v>35147615</v>
       </c>
     </row>
     <row r="22">
@@ -1620,13 +1620,13 @@
         <v>90.3563</v>
       </c>
       <c r="D22" t="n">
-        <v>330724.455823293</v>
+        <v>331676.871743487</v>
       </c>
       <c r="E22" t="n">
-        <v>330724.455823293</v>
+        <v>331676.871743487</v>
       </c>
       <c r="F22" t="n">
-        <v>164700779</v>
+        <v>165506759</v>
       </c>
     </row>
     <row r="23">
@@ -1640,13 +1640,13 @@
         <v>-59.5432</v>
       </c>
       <c r="D23" t="n">
-        <v>985.614457831325</v>
+        <v>991.707414829659</v>
       </c>
       <c r="E23" t="n">
-        <v>985.614457831325</v>
+        <v>991.707414829659</v>
       </c>
       <c r="F23" t="n">
-        <v>490836</v>
+        <v>494862</v>
       </c>
     </row>
     <row r="24">
@@ -1660,13 +1660,13 @@
         <v>27.9534</v>
       </c>
       <c r="D24" t="n">
-        <v>134570.050200803</v>
+        <v>135095.699398798</v>
       </c>
       <c r="E24" t="n">
-        <v>134570.050200803</v>
+        <v>135095.699398798</v>
       </c>
       <c r="F24" t="n">
-        <v>67015885</v>
+        <v>67412754</v>
       </c>
     </row>
     <row r="25">
@@ -1680,13 +1680,13 @@
         <v>4.469936</v>
       </c>
       <c r="D25" t="n">
-        <v>367995.871485944</v>
+        <v>369396.595190381</v>
       </c>
       <c r="E25" t="n">
-        <v>367995.871485944</v>
+        <v>369396.595190381</v>
       </c>
       <c r="F25" t="n">
-        <v>183261944</v>
+        <v>184328901</v>
       </c>
     </row>
     <row r="26">
@@ -1700,13 +1700,13 @@
         <v>-88.4976</v>
       </c>
       <c r="D26" t="n">
-        <v>4920.89156626506</v>
+        <v>4936.76152304609</v>
       </c>
       <c r="E26" t="n">
-        <v>4920.89156626506</v>
+        <v>4936.76152304609</v>
       </c>
       <c r="F26" t="n">
-        <v>2450604</v>
+        <v>2463444</v>
       </c>
     </row>
     <row r="27">
@@ -1720,13 +1720,13 @@
         <v>2.3158</v>
       </c>
       <c r="D27" t="n">
-        <v>2806.66265060241</v>
+        <v>2817.23446893788</v>
       </c>
       <c r="E27" t="n">
-        <v>2806.66265060241</v>
+        <v>2817.23446893788</v>
       </c>
       <c r="F27" t="n">
-        <v>1397718</v>
+        <v>1405800</v>
       </c>
     </row>
     <row r="28">
@@ -1740,13 +1740,13 @@
         <v>90.4336</v>
       </c>
       <c r="D28" t="n">
-        <v>406.789156626506</v>
+        <v>409.288577154309</v>
       </c>
       <c r="E28" t="n">
-        <v>406.789156626506</v>
+        <v>409.288577154309</v>
       </c>
       <c r="F28" t="n">
-        <v>202581</v>
+        <v>204235</v>
       </c>
     </row>
     <row r="29">
@@ -1760,13 +1760,13 @@
         <v>-63.5887</v>
       </c>
       <c r="D29" t="n">
-        <v>126183.303212851</v>
+        <v>126692.869739479</v>
       </c>
       <c r="E29" t="n">
-        <v>126183.303212851</v>
+        <v>126692.869739479</v>
       </c>
       <c r="F29" t="n">
-        <v>62839285</v>
+        <v>63219742</v>
       </c>
     </row>
     <row r="30">
@@ -1780,13 +1780,13 @@
         <v>17.6791</v>
       </c>
       <c r="D30" t="n">
-        <v>64403.9116465863</v>
+        <v>64684.1683366733</v>
       </c>
       <c r="E30" t="n">
-        <v>64403.9116465863</v>
+        <v>64684.1683366733</v>
       </c>
       <c r="F30" t="n">
-        <v>32073148</v>
+        <v>32277400</v>
       </c>
     </row>
     <row r="31">
@@ -1800,13 +1800,13 @@
         <v>24.6849</v>
       </c>
       <c r="D31" t="n">
-        <v>12614.6907630522</v>
+        <v>12702.0701402806</v>
       </c>
       <c r="E31" t="n">
-        <v>12614.6907630522</v>
+        <v>12702.0701402806</v>
       </c>
       <c r="F31" t="n">
-        <v>6282116</v>
+        <v>6338333</v>
       </c>
     </row>
     <row r="32">
@@ -1820,13 +1820,13 @@
         <v>-51.9253</v>
       </c>
       <c r="D32" t="n">
-        <v>5461899.08433735</v>
+        <v>5484627.68737475</v>
       </c>
       <c r="E32" t="n">
-        <v>5461899.08433735</v>
+        <v>5484627.68737475</v>
       </c>
       <c r="F32" t="n">
-        <v>2720025744</v>
+        <v>2736829216</v>
       </c>
     </row>
     <row r="33">
@@ -1840,13 +1840,13 @@
         <v>114.7277</v>
       </c>
       <c r="D33" t="n">
-        <v>144.979919678715</v>
+        <v>145.178356713427</v>
       </c>
       <c r="E33" t="n">
-        <v>144.979919678715</v>
+        <v>145.178356713427</v>
       </c>
       <c r="F33" t="n">
-        <v>72200</v>
+        <v>72444</v>
       </c>
     </row>
     <row r="34">
@@ -1860,13 +1860,13 @@
         <v>25.4858</v>
       </c>
       <c r="D34" t="n">
-        <v>116876.939759036</v>
+        <v>117482.75751503</v>
       </c>
       <c r="E34" t="n">
-        <v>116876.939759036</v>
+        <v>117482.75751503</v>
       </c>
       <c r="F34" t="n">
-        <v>58204716</v>
+        <v>58623896</v>
       </c>
     </row>
     <row r="35">
@@ -1880,13 +1880,13 @@
         <v>-1.5616</v>
       </c>
       <c r="D35" t="n">
-        <v>4624.5983935743</v>
+        <v>4642.27655310621</v>
       </c>
       <c r="E35" t="n">
-        <v>4624.5983935743</v>
+        <v>4642.27655310621</v>
       </c>
       <c r="F35" t="n">
-        <v>2303050</v>
+        <v>2316496</v>
       </c>
     </row>
     <row r="36">
@@ -1900,13 +1900,13 @@
         <v>95.956</v>
       </c>
       <c r="D36" t="n">
-        <v>56812.09437751</v>
+        <v>56986.7094188377</v>
       </c>
       <c r="E36" t="n">
-        <v>56812.09437751</v>
+        <v>56986.7094188377</v>
       </c>
       <c r="F36" t="n">
-        <v>28292423</v>
+        <v>28436368</v>
       </c>
     </row>
     <row r="37">
@@ -1920,13 +1920,13 @@
         <v>29.9189</v>
       </c>
       <c r="D37" t="n">
-        <v>1027.90562248996</v>
+        <v>1035.55310621242</v>
       </c>
       <c r="E37" t="n">
-        <v>1027.90562248996</v>
+        <v>1035.55310621242</v>
       </c>
       <c r="F37" t="n">
-        <v>511897</v>
+        <v>516741</v>
       </c>
     </row>
     <row r="38">
@@ -1940,13 +1940,13 @@
         <v>-23.0418</v>
       </c>
       <c r="D38" t="n">
-        <v>8158.83534136546</v>
+        <v>8204.15631262525</v>
       </c>
       <c r="E38" t="n">
-        <v>8158.83534136546</v>
+        <v>8204.15631262525</v>
       </c>
       <c r="F38" t="n">
-        <v>4063100</v>
+        <v>4093874</v>
       </c>
     </row>
     <row r="39">
@@ -1960,13 +1960,13 @@
         <v>104.9167</v>
       </c>
       <c r="D39" t="n">
-        <v>2163.79317269076</v>
+        <v>2223.96392785571</v>
       </c>
       <c r="E39" t="n">
-        <v>2163.79317269076</v>
+        <v>2223.96392785571</v>
       </c>
       <c r="F39" t="n">
-        <v>1077569</v>
+        <v>1109758</v>
       </c>
     </row>
     <row r="40">
@@ -1980,13 +1980,13 @@
         <v>11.5021</v>
       </c>
       <c r="D40" t="n">
-        <v>23418.2831325301</v>
+        <v>23529.5270541082</v>
       </c>
       <c r="E40" t="n">
-        <v>23418.2831325301</v>
+        <v>23529.5270541082</v>
       </c>
       <c r="F40" t="n">
-        <v>11662305</v>
+        <v>11741234</v>
       </c>
     </row>
     <row r="41">
@@ -2000,13 +2000,13 @@
         <v>-116.5765</v>
       </c>
       <c r="D41" t="n">
-        <v>59867.2168674699</v>
+        <v>60205.006012024</v>
       </c>
       <c r="E41" t="n">
-        <v>59867.2168674699</v>
+        <v>60205.006012024</v>
       </c>
       <c r="F41" t="n">
-        <v>29813874</v>
+        <v>30042298</v>
       </c>
     </row>
     <row r="42">
@@ -2020,13 +2020,13 @@
         <v>-127.6476</v>
       </c>
       <c r="D42" t="n">
-        <v>35705.9397590361</v>
+        <v>35924.6973947896</v>
       </c>
       <c r="E42" t="n">
-        <v>35705.9397590361</v>
+        <v>35924.6973947896</v>
       </c>
       <c r="F42" t="n">
-        <v>17781558</v>
+        <v>17926424</v>
       </c>
     </row>
     <row r="43">
@@ -2040,10 +2040,10 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0642570281124498</v>
+        <v>0.064128256513026</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0642570281124498</v>
+        <v>0.064128256513026</v>
       </c>
       <c r="F43" t="n">
         <v>32</v>
@@ -2060,13 +2060,13 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>11.5421686746988</v>
+        <v>11.5450901803607</v>
       </c>
       <c r="E44" t="n">
-        <v>11.5421686746988</v>
+        <v>11.5450901803607</v>
       </c>
       <c r="F44" t="n">
-        <v>5748</v>
+        <v>5761</v>
       </c>
     </row>
     <row r="45">
@@ -2080,13 +2080,13 @@
         <v>-98.8139</v>
       </c>
       <c r="D45" t="n">
-        <v>13084.9156626506</v>
+        <v>13162.7715430862</v>
       </c>
       <c r="E45" t="n">
-        <v>13084.9156626506</v>
+        <v>13162.7715430862</v>
       </c>
       <c r="F45" t="n">
-        <v>6516288</v>
+        <v>6568223</v>
       </c>
     </row>
     <row r="46">
@@ -2100,13 +2100,13 @@
         <v>-66.4619</v>
       </c>
       <c r="D46" t="n">
-        <v>606.327309236948</v>
+        <v>609.607214428858</v>
       </c>
       <c r="E46" t="n">
-        <v>606.327309236948</v>
+        <v>609.607214428858</v>
       </c>
       <c r="F46" t="n">
-        <v>301951</v>
+        <v>304194</v>
       </c>
     </row>
     <row r="47">
@@ -2120,13 +2120,13 @@
         <v>-57.6604</v>
       </c>
       <c r="D47" t="n">
-        <v>425.335341365462</v>
+        <v>427.168336673347</v>
       </c>
       <c r="E47" t="n">
-        <v>425.335341365462</v>
+        <v>427.168336673347</v>
       </c>
       <c r="F47" t="n">
-        <v>211817</v>
+        <v>213157</v>
       </c>
     </row>
     <row r="48">
@@ -2140,13 +2140,13 @@
         <v>-124.8457</v>
       </c>
       <c r="D48" t="n">
-        <v>21.8935742971888</v>
+        <v>22.1062124248497</v>
       </c>
       <c r="E48" t="n">
-        <v>21.8935742971888</v>
+        <v>22.1062124248497</v>
       </c>
       <c r="F48" t="n">
-        <v>10903</v>
+        <v>11031</v>
       </c>
     </row>
     <row r="49">
@@ -2160,13 +2160,13 @@
         <v>-63.7443</v>
       </c>
       <c r="D49" t="n">
-        <v>1294.86746987952</v>
+        <v>1303.53106212425</v>
       </c>
       <c r="E49" t="n">
-        <v>1294.86746987952</v>
+        <v>1303.53106212425</v>
       </c>
       <c r="F49" t="n">
-        <v>644844</v>
+        <v>650462</v>
       </c>
     </row>
     <row r="50">
@@ -2180,13 +2180,13 @@
         <v>-83.1076</v>
       </c>
       <c r="D50" t="n">
-        <v>143.194779116466</v>
+        <v>144.206412825651</v>
       </c>
       <c r="E50" t="n">
-        <v>143.194779116466</v>
+        <v>144.206412825651</v>
       </c>
       <c r="F50" t="n">
-        <v>71311</v>
+        <v>71959</v>
       </c>
     </row>
     <row r="51">
@@ -2200,13 +2200,13 @@
         <v>-85.3232</v>
       </c>
       <c r="D51" t="n">
-        <v>142038.634538153</v>
+        <v>142839.440881764</v>
       </c>
       <c r="E51" t="n">
-        <v>142038.634538153</v>
+        <v>142839.440881764</v>
       </c>
       <c r="F51" t="n">
-        <v>70735240</v>
+        <v>71276881</v>
       </c>
     </row>
     <row r="52">
@@ -2220,13 +2220,13 @@
         <v>-63.4168</v>
       </c>
       <c r="D52" t="n">
-        <v>70.9879518072289</v>
+        <v>71.2545090180361</v>
       </c>
       <c r="E52" t="n">
-        <v>70.9879518072289</v>
+        <v>71.2545090180361</v>
       </c>
       <c r="F52" t="n">
-        <v>35352</v>
+        <v>35556</v>
       </c>
     </row>
     <row r="53">
@@ -2240,13 +2240,13 @@
         <v>-73.5491</v>
       </c>
       <c r="D53" t="n">
-        <v>134954.293172691</v>
+        <v>135427.49498998</v>
       </c>
       <c r="E53" t="n">
-        <v>134954.293172691</v>
+        <v>135427.49498998</v>
       </c>
       <c r="F53" t="n">
-        <v>67207238</v>
+        <v>67578320</v>
       </c>
     </row>
     <row r="54">
@@ -2256,13 +2256,13 @@
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" t="n">
-        <v>4.9859437751004</v>
+        <v>5.00200400801603</v>
       </c>
       <c r="E54" t="n">
-        <v>4.9859437751004</v>
+        <v>5.00200400801603</v>
       </c>
       <c r="F54" t="n">
-        <v>2483</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="55">
@@ -2276,13 +2276,13 @@
         <v>-106.4509</v>
       </c>
       <c r="D55" t="n">
-        <v>11454.9036144578</v>
+        <v>11526.3306613226</v>
       </c>
       <c r="E55" t="n">
-        <v>11454.9036144578</v>
+        <v>11526.3306613226</v>
       </c>
       <c r="F55" t="n">
-        <v>5704542</v>
+        <v>5751639</v>
       </c>
     </row>
     <row r="56">
@@ -2296,13 +2296,13 @@
         <v>-135</v>
       </c>
       <c r="D56" t="n">
-        <v>33.8152610441767</v>
+        <v>33.9158316633267</v>
       </c>
       <c r="E56" t="n">
-        <v>33.8152610441767</v>
+        <v>33.9158316633267</v>
       </c>
       <c r="F56" t="n">
-        <v>16840</v>
+        <v>16924</v>
       </c>
     </row>
     <row r="57">
@@ -2316,13 +2316,13 @@
         <v>20.9394</v>
       </c>
       <c r="D57" t="n">
-        <v>3624.87751004016</v>
+        <v>3631.82364729459</v>
       </c>
       <c r="E57" t="n">
-        <v>3624.87751004016</v>
+        <v>3631.82364729459</v>
       </c>
       <c r="F57" t="n">
-        <v>1805189</v>
+        <v>1812280</v>
       </c>
     </row>
     <row r="58">
@@ -2336,13 +2336,13 @@
         <v>18.7322</v>
       </c>
       <c r="D58" t="n">
-        <v>1814.1686746988</v>
+        <v>1820.42284569138</v>
       </c>
       <c r="E58" t="n">
-        <v>1814.1686746988</v>
+        <v>1820.42284569138</v>
       </c>
       <c r="F58" t="n">
-        <v>903456</v>
+        <v>908391</v>
       </c>
     </row>
     <row r="59">
@@ -2356,13 +2356,13 @@
         <v>-71.543</v>
       </c>
       <c r="D59" t="n">
-        <v>479456.337349398</v>
+        <v>481307.328657315</v>
       </c>
       <c r="E59" t="n">
-        <v>479456.337349398</v>
+        <v>481307.328657315</v>
       </c>
       <c r="F59" t="n">
-        <v>238769256</v>
+        <v>240172357</v>
       </c>
     </row>
     <row r="60">
@@ -2376,13 +2376,13 @@
         <v>117.2264</v>
       </c>
       <c r="D60" t="n">
-        <v>964.606425702811</v>
+        <v>964.685370741483</v>
       </c>
       <c r="E60" t="n">
-        <v>964.606425702811</v>
+        <v>964.685370741483</v>
       </c>
       <c r="F60" t="n">
-        <v>480374</v>
+        <v>481378</v>
       </c>
     </row>
     <row r="61">
@@ -2396,13 +2396,13 @@
         <v>116.4142</v>
       </c>
       <c r="D61" t="n">
-        <v>835.779116465863</v>
+        <v>836.230460921844</v>
       </c>
       <c r="E61" t="n">
-        <v>835.779116465863</v>
+        <v>836.230460921844</v>
       </c>
       <c r="F61" t="n">
-        <v>416218</v>
+        <v>417279</v>
       </c>
     </row>
     <row r="62">
@@ -2416,13 +2416,13 @@
         <v>107.874</v>
       </c>
       <c r="D62" t="n">
-        <v>571.273092369478</v>
+        <v>571.326653306613</v>
       </c>
       <c r="E62" t="n">
-        <v>571.273092369478</v>
+        <v>571.326653306613</v>
       </c>
       <c r="F62" t="n">
-        <v>284494</v>
+        <v>285092</v>
       </c>
     </row>
     <row r="63">
@@ -2436,13 +2436,13 @@
         <v>117.9874</v>
       </c>
       <c r="D63" t="n">
-        <v>428.759036144578</v>
+        <v>429.152304609218</v>
       </c>
       <c r="E63" t="n">
-        <v>428.759036144578</v>
+        <v>429.152304609218</v>
       </c>
       <c r="F63" t="n">
-        <v>213522</v>
+        <v>214147</v>
       </c>
     </row>
     <row r="64">
@@ -2456,13 +2456,13 @@
         <v>104.2861</v>
       </c>
       <c r="D64" t="n">
-        <v>160.744979919679</v>
+        <v>160.811623246493</v>
       </c>
       <c r="E64" t="n">
-        <v>160.744979919679</v>
+        <v>160.811623246493</v>
       </c>
       <c r="F64" t="n">
-        <v>80051</v>
+        <v>80245</v>
       </c>
     </row>
     <row r="65">
@@ -2476,13 +2476,13 @@
         <v>113.4244</v>
       </c>
       <c r="D65" t="n">
-        <v>1817.13453815261</v>
+        <v>1818.52104208417</v>
       </c>
       <c r="E65" t="n">
-        <v>1817.13453815261</v>
+        <v>1818.52104208417</v>
       </c>
       <c r="F65" t="n">
-        <v>904933</v>
+        <v>907442</v>
       </c>
     </row>
     <row r="66">
@@ -2496,13 +2496,13 @@
         <v>108.7881</v>
       </c>
       <c r="D66" t="n">
-        <v>253.471887550201</v>
+        <v>253.51503006012</v>
       </c>
       <c r="E66" t="n">
-        <v>253.471887550201</v>
+        <v>253.51503006012</v>
       </c>
       <c r="F66" t="n">
-        <v>126229</v>
+        <v>126504</v>
       </c>
     </row>
     <row r="67">
@@ -2516,13 +2516,13 @@
         <v>106.8748</v>
       </c>
       <c r="D67" t="n">
-        <v>142.39156626506</v>
+        <v>142.400801603206</v>
       </c>
       <c r="E67" t="n">
-        <v>142.39156626506</v>
+        <v>142.400801603206</v>
       </c>
       <c r="F67" t="n">
-        <v>70911</v>
+        <v>71058</v>
       </c>
     </row>
     <row r="68">
@@ -2536,13 +2536,13 @@
         <v>109.7453</v>
       </c>
       <c r="D68" t="n">
-        <v>167.35140562249</v>
+        <v>167.392785571142</v>
       </c>
       <c r="E68" t="n">
-        <v>167.35140562249</v>
+        <v>167.392785571142</v>
       </c>
       <c r="F68" t="n">
-        <v>83341</v>
+        <v>83529</v>
       </c>
     </row>
     <row r="69">
@@ -2556,13 +2556,13 @@
         <v>116.1306</v>
       </c>
       <c r="D69" t="n">
-        <v>610.427710843373</v>
+        <v>611.843687374749</v>
       </c>
       <c r="E69" t="n">
-        <v>610.427710843373</v>
+        <v>611.843687374749</v>
       </c>
       <c r="F69" t="n">
-        <v>303993</v>
+        <v>305310</v>
       </c>
     </row>
     <row r="70">
@@ -2576,13 +2576,13 @@
         <v>127.7615</v>
       </c>
       <c r="D70" t="n">
-        <v>1032.31726907631</v>
+        <v>1033.47895791583</v>
       </c>
       <c r="E70" t="n">
-        <v>1032.31726907631</v>
+        <v>1033.47895791583</v>
       </c>
       <c r="F70" t="n">
-        <v>514094</v>
+        <v>515706</v>
       </c>
     </row>
     <row r="71">
@@ -2596,13 +2596,13 @@
         <v>114.9042</v>
       </c>
       <c r="D71" t="n">
-        <v>1253.41967871486</v>
+        <v>1253.54308617234</v>
       </c>
       <c r="E71" t="n">
-        <v>1253.41967871486</v>
+        <v>1253.54308617234</v>
       </c>
       <c r="F71" t="n">
-        <v>624203</v>
+        <v>625518</v>
       </c>
     </row>
     <row r="72">
@@ -2616,13 +2616,13 @@
         <v>114.2</v>
       </c>
       <c r="D72" t="n">
-        <v>5429.87951807229</v>
+        <v>5442.74348697395</v>
       </c>
       <c r="E72" t="n">
-        <v>5429.87951807229</v>
+        <v>5442.74348697395</v>
       </c>
       <c r="F72" t="n">
-        <v>2704080</v>
+        <v>2715929</v>
       </c>
     </row>
     <row r="73">
@@ -2636,13 +2636,13 @@
         <v>112.2707</v>
       </c>
       <c r="D73" t="n">
-        <v>65456.8072289157</v>
+        <v>65462.2224448898</v>
       </c>
       <c r="E73" t="n">
-        <v>65456.8072289157</v>
+        <v>65462.2224448898</v>
       </c>
       <c r="F73" t="n">
-        <v>32597490</v>
+        <v>32665649</v>
       </c>
     </row>
     <row r="74">
@@ -2656,13 +2656,13 @@
         <v>111.7088</v>
       </c>
       <c r="D74" t="n">
-        <v>998.971887550201</v>
+        <v>999.076152304609</v>
       </c>
       <c r="E74" t="n">
-        <v>998.971887550201</v>
+        <v>999.076152304609</v>
       </c>
       <c r="F74" t="n">
-        <v>497488</v>
+        <v>498539</v>
       </c>
     </row>
     <row r="75">
@@ -2676,13 +2676,13 @@
         <v>113.9448</v>
       </c>
       <c r="D75" t="n">
-        <v>265.44578313253</v>
+        <v>265.691382765531</v>
       </c>
       <c r="E75" t="n">
-        <v>265.44578313253</v>
+        <v>265.691382765531</v>
       </c>
       <c r="F75" t="n">
-        <v>132192</v>
+        <v>132580</v>
       </c>
     </row>
     <row r="76">
@@ -2696,13 +2696,13 @@
         <v>119.455</v>
       </c>
       <c r="D76" t="n">
-        <v>654.558232931727</v>
+        <v>654.703406813627</v>
       </c>
       <c r="E76" t="n">
-        <v>654.558232931727</v>
+        <v>654.703406813627</v>
       </c>
       <c r="F76" t="n">
-        <v>325970</v>
+        <v>326697</v>
       </c>
     </row>
     <row r="77">
@@ -2716,13 +2716,13 @@
         <v>115.7221</v>
       </c>
       <c r="D77" t="n">
-        <v>909.419678714859</v>
+        <v>909.4749498998</v>
       </c>
       <c r="E77" t="n">
-        <v>909.419678714859</v>
+        <v>909.4749498998</v>
       </c>
       <c r="F77" t="n">
-        <v>452891</v>
+        <v>453828</v>
       </c>
     </row>
     <row r="78">
@@ -2736,13 +2736,13 @@
         <v>126.1923</v>
       </c>
       <c r="D78" t="n">
-        <v>249.674698795181</v>
+        <v>250.322645290581</v>
       </c>
       <c r="E78" t="n">
-        <v>249.674698795181</v>
+        <v>250.322645290581</v>
       </c>
       <c r="F78" t="n">
-        <v>124338</v>
+        <v>124911</v>
       </c>
     </row>
     <row r="79">
@@ -2756,13 +2756,13 @@
         <v>122.6085</v>
       </c>
       <c r="D79" t="n">
-        <v>262.588353413655</v>
+        <v>262.913827655311</v>
       </c>
       <c r="E79" t="n">
-        <v>262.588353413655</v>
+        <v>262.913827655311</v>
       </c>
       <c r="F79" t="n">
-        <v>130769</v>
+        <v>131194</v>
       </c>
     </row>
     <row r="80">
@@ -2776,13 +2776,13 @@
         <v>113.55</v>
       </c>
       <c r="D80" t="n">
-        <v>41.7931726907631</v>
+        <v>41.811623246493</v>
       </c>
       <c r="E80" t="n">
-        <v>41.7931726907631</v>
+        <v>41.811623246493</v>
       </c>
       <c r="F80" t="n">
-        <v>20813</v>
+        <v>20864</v>
       </c>
     </row>
     <row r="81">
@@ -2796,13 +2796,13 @@
         <v>106.1655</v>
       </c>
       <c r="D81" t="n">
-        <v>72.7068273092369</v>
+        <v>72.7134268537074</v>
       </c>
       <c r="E81" t="n">
-        <v>72.7068273092369</v>
+        <v>72.7134268537074</v>
       </c>
       <c r="F81" t="n">
-        <v>36208</v>
+        <v>36284</v>
       </c>
     </row>
     <row r="82">
@@ -2816,13 +2816,13 @@
         <v>95.9956</v>
       </c>
       <c r="D82" t="n">
-        <v>17.6606425702811</v>
+        <v>17.6613226452906</v>
       </c>
       <c r="E82" t="n">
-        <v>17.6606425702811</v>
+        <v>17.6613226452906</v>
       </c>
       <c r="F82" t="n">
-        <v>8795</v>
+        <v>8813</v>
       </c>
     </row>
     <row r="83">
@@ -2836,13 +2836,13 @@
         <v>108.8701</v>
       </c>
       <c r="D83" t="n">
-        <v>408.455823293173</v>
+        <v>408.87374749499</v>
       </c>
       <c r="E83" t="n">
-        <v>408.455823293173</v>
+        <v>408.87374749499</v>
       </c>
       <c r="F83" t="n">
-        <v>203411</v>
+        <v>204028</v>
       </c>
     </row>
     <row r="84">
@@ -2856,13 +2856,13 @@
         <v>118.1498</v>
       </c>
       <c r="D84" t="n">
-        <v>799.144578313253</v>
+        <v>799.312625250501</v>
       </c>
       <c r="E84" t="n">
-        <v>799.144578313253</v>
+        <v>799.312625250501</v>
       </c>
       <c r="F84" t="n">
-        <v>397974</v>
+        <v>398857</v>
       </c>
     </row>
     <row r="85">
@@ -2876,13 +2876,13 @@
         <v>121.4491</v>
       </c>
       <c r="D85" t="n">
-        <v>1114.68875502008</v>
+        <v>1116.69539078156</v>
       </c>
       <c r="E85" t="n">
-        <v>1114.68875502008</v>
+        <v>1116.69539078156</v>
       </c>
       <c r="F85" t="n">
-        <v>555115</v>
+        <v>557231</v>
       </c>
     </row>
     <row r="86">
@@ -2896,13 +2896,13 @@
         <v>112.2922</v>
       </c>
       <c r="D86" t="n">
-        <v>201.839357429719</v>
+        <v>201.941883767535</v>
       </c>
       <c r="E86" t="n">
-        <v>201.839357429719</v>
+        <v>201.941883767535</v>
       </c>
       <c r="F86" t="n">
-        <v>100516</v>
+        <v>100769</v>
       </c>
     </row>
     <row r="87">
@@ -2916,13 +2916,13 @@
         <v>102.7103</v>
       </c>
       <c r="D87" t="n">
-        <v>711.0140562249</v>
+        <v>711.657314629259</v>
       </c>
       <c r="E87" t="n">
-        <v>711.0140562249</v>
+        <v>711.657314629259</v>
       </c>
       <c r="F87" t="n">
-        <v>354085</v>
+        <v>355117</v>
       </c>
     </row>
     <row r="88">
@@ -2936,13 +2936,13 @@
         <v>117.323</v>
       </c>
       <c r="D88" t="n">
-        <v>253.598393574297</v>
+        <v>253.877755511022</v>
       </c>
       <c r="E88" t="n">
-        <v>253.598393574297</v>
+        <v>253.877755511022</v>
       </c>
       <c r="F88" t="n">
-        <v>126292</v>
+        <v>126685</v>
       </c>
     </row>
     <row r="89">
@@ -2956,13 +2956,13 @@
         <v>88.0924</v>
       </c>
       <c r="D89" t="n">
-        <v>0.983935742971888</v>
+        <v>0.983967935871743</v>
       </c>
       <c r="E89" t="n">
-        <v>0.983935742971888</v>
+        <v>0.983967935871743</v>
       </c>
       <c r="F89" t="n">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="90">
@@ -2972,10 +2972,10 @@
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90" t="n">
-        <v>0.0140562248995984</v>
+        <v>0.0140280561122244</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0140562248995984</v>
+        <v>0.0140280561122244</v>
       </c>
       <c r="F90" t="n">
         <v>7</v>
@@ -2992,13 +2992,13 @@
         <v>85.2401</v>
       </c>
       <c r="D91" t="n">
-        <v>618.220883534137</v>
+        <v>618.945891783567</v>
       </c>
       <c r="E91" t="n">
-        <v>618.220883534137</v>
+        <v>618.945891783567</v>
       </c>
       <c r="F91" t="n">
-        <v>307874</v>
+        <v>308854</v>
       </c>
     </row>
     <row r="92">
@@ -3012,13 +3012,13 @@
         <v>101.487</v>
       </c>
       <c r="D92" t="n">
-        <v>215.008032128514</v>
+        <v>215.288577154309</v>
       </c>
       <c r="E92" t="n">
-        <v>215.008032128514</v>
+        <v>215.288577154309</v>
       </c>
       <c r="F92" t="n">
-        <v>107074</v>
+        <v>107429</v>
       </c>
     </row>
     <row r="93">
@@ -3032,13 +3032,13 @@
         <v>120.0934</v>
       </c>
       <c r="D93" t="n">
-        <v>1256.4437751004</v>
+        <v>1256.66132264529</v>
       </c>
       <c r="E93" t="n">
-        <v>1256.4437751004</v>
+        <v>1256.66132264529</v>
       </c>
       <c r="F93" t="n">
-        <v>625709</v>
+        <v>627074</v>
       </c>
     </row>
     <row r="94">
@@ -3052,13 +3052,13 @@
         <v>-74.2973</v>
       </c>
       <c r="D94" t="n">
-        <v>1062614.61044177</v>
+        <v>1067475.19438878</v>
       </c>
       <c r="E94" t="n">
-        <v>1062614.61044177</v>
+        <v>1067475.19438878</v>
       </c>
       <c r="F94" t="n">
-        <v>529182076</v>
+        <v>532670122</v>
       </c>
     </row>
     <row r="95">
@@ -3072,13 +3072,13 @@
         <v>43.3333</v>
       </c>
       <c r="D95" t="n">
-        <v>1195.24096385542</v>
+        <v>1200.625250501</v>
       </c>
       <c r="E95" t="n">
-        <v>1195.24096385542</v>
+        <v>1200.625250501</v>
       </c>
       <c r="F95" t="n">
-        <v>595230</v>
+        <v>599112</v>
       </c>
     </row>
     <row r="96">
@@ -3092,13 +3092,13 @@
         <v>15.8277</v>
       </c>
       <c r="D96" t="n">
-        <v>4685.88152610442</v>
+        <v>4700.22845691383</v>
       </c>
       <c r="E96" t="n">
-        <v>4685.88152610442</v>
+        <v>4700.22845691383</v>
       </c>
       <c r="F96" t="n">
-        <v>2333569</v>
+        <v>2345414</v>
       </c>
     </row>
     <row r="97">
@@ -3112,13 +3112,13 @@
         <v>21.7587</v>
       </c>
       <c r="D97" t="n">
-        <v>12601.0682730924</v>
+        <v>12640.2985971944</v>
       </c>
       <c r="E97" t="n">
-        <v>12601.0682730924</v>
+        <v>12640.2985971944</v>
       </c>
       <c r="F97" t="n">
-        <v>6275332</v>
+        <v>6307509</v>
       </c>
     </row>
     <row r="98">
@@ -3132,13 +3132,13 @@
         <v>-83.7534</v>
       </c>
       <c r="D98" t="n">
-        <v>97738.5602409639</v>
+        <v>98195.5551102204</v>
       </c>
       <c r="E98" t="n">
-        <v>97738.5602409639</v>
+        <v>98195.5551102204</v>
       </c>
       <c r="F98" t="n">
-        <v>48673803</v>
+        <v>48999582</v>
       </c>
     </row>
     <row r="99">
@@ -3152,13 +3152,13 @@
         <v>-5.5471</v>
       </c>
       <c r="D99" t="n">
-        <v>18960.3072289157</v>
+        <v>19017.2785571142</v>
       </c>
       <c r="E99" t="n">
-        <v>18960.3072289157</v>
+        <v>19017.2785571142</v>
       </c>
       <c r="F99" t="n">
-        <v>9442233</v>
+        <v>9489622</v>
       </c>
     </row>
     <row r="100">
@@ -3172,13 +3172,13 @@
         <v>15.2</v>
       </c>
       <c r="D100" t="n">
-        <v>104330.710843373</v>
+        <v>104837.280561122</v>
       </c>
       <c r="E100" t="n">
-        <v>104330.710843373</v>
+        <v>104837.280561122</v>
       </c>
       <c r="F100" t="n">
-        <v>51956694</v>
+        <v>52313803</v>
       </c>
     </row>
     <row r="101">
@@ -3192,13 +3192,13 @@
         <v>-77.781167</v>
       </c>
       <c r="D101" t="n">
-        <v>23456.5662650602</v>
+        <v>23701.2765531062</v>
       </c>
       <c r="E101" t="n">
-        <v>23456.5662650602</v>
+        <v>23701.2765531062</v>
       </c>
       <c r="F101" t="n">
-        <v>11681370</v>
+        <v>11826937</v>
       </c>
     </row>
     <row r="102">
@@ -3212,13 +3212,13 @@
         <v>33.4299</v>
       </c>
       <c r="D102" t="n">
-        <v>16116.5421686747</v>
+        <v>16229.7875751503</v>
       </c>
       <c r="E102" t="n">
-        <v>16116.5421686747</v>
+        <v>16229.7875751503</v>
       </c>
       <c r="F102" t="n">
-        <v>8026038</v>
+        <v>8098664</v>
       </c>
     </row>
     <row r="103">
@@ -3232,13 +3232,13 @@
         <v>15.473</v>
       </c>
       <c r="D103" t="n">
-        <v>490982.002008032</v>
+        <v>493329.9498998</v>
       </c>
       <c r="E103" t="n">
-        <v>490982.002008032</v>
+        <v>493329.9498998</v>
       </c>
       <c r="F103" t="n">
-        <v>244509037</v>
+        <v>246171645</v>
       </c>
     </row>
     <row r="104">
@@ -3252,13 +3252,13 @@
         <v>-6.9118</v>
       </c>
       <c r="D104" t="n">
-        <v>394.022088353414</v>
+        <v>394.697394789579</v>
       </c>
       <c r="E104" t="n">
-        <v>394.022088353414</v>
+        <v>394.697394789579</v>
       </c>
       <c r="F104" t="n">
-        <v>196223</v>
+        <v>196954</v>
       </c>
     </row>
     <row r="105">
@@ -3272,13 +3272,13 @@
         <v>-42.6043</v>
       </c>
       <c r="D105" t="n">
-        <v>17.7248995983936</v>
+        <v>17.7695390781563</v>
       </c>
       <c r="E105" t="n">
-        <v>17.7248995983936</v>
+        <v>17.7695390781563</v>
       </c>
       <c r="F105" t="n">
-        <v>8827</v>
+        <v>8867</v>
       </c>
     </row>
     <row r="106">
@@ -3292,13 +3292,13 @@
         <v>9.5018</v>
       </c>
       <c r="D106" t="n">
-        <v>87600.7530120482</v>
+        <v>87994.5731462926</v>
       </c>
       <c r="E106" t="n">
-        <v>87600.7530120482</v>
+        <v>87994.5731462926</v>
       </c>
       <c r="F106" t="n">
-        <v>43625175</v>
+        <v>43909292</v>
       </c>
     </row>
     <row r="107">
@@ -3312,13 +3312,13 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>676.265060240964</v>
+        <v>676.336673346693</v>
       </c>
       <c r="E107" t="n">
-        <v>676.265060240964</v>
+        <v>676.336673346693</v>
       </c>
       <c r="F107" t="n">
-        <v>336780</v>
+        <v>337492</v>
       </c>
     </row>
     <row r="108">
@@ -3332,13 +3332,13 @@
         <v>42.5903</v>
       </c>
       <c r="D108" t="n">
-        <v>4885.88353413655</v>
+        <v>4899.22645290581</v>
       </c>
       <c r="E108" t="n">
-        <v>4885.88353413655</v>
+        <v>4899.22645290581</v>
       </c>
       <c r="F108" t="n">
-        <v>2433170</v>
+        <v>2444714</v>
       </c>
     </row>
     <row r="109">
@@ -3352,13 +3352,13 @@
         <v>-61.371</v>
       </c>
       <c r="D109" t="n">
-        <v>64.0421686746988</v>
+        <v>64.2905811623247</v>
       </c>
       <c r="E109" t="n">
-        <v>64.0421686746988</v>
+        <v>64.2905811623247</v>
       </c>
       <c r="F109" t="n">
-        <v>31893</v>
+        <v>32081</v>
       </c>
     </row>
     <row r="110">
@@ -3372,13 +3372,13 @@
         <v>-70.1627</v>
       </c>
       <c r="D110" t="n">
-        <v>116816.730923695</v>
+        <v>117178.058116232</v>
       </c>
       <c r="E110" t="n">
-        <v>116816.730923695</v>
+        <v>117178.058116232</v>
       </c>
       <c r="F110" t="n">
-        <v>58174732</v>
+        <v>58471851</v>
       </c>
     </row>
     <row r="111">
@@ -3392,13 +3392,13 @@
         <v>-78.1834</v>
       </c>
       <c r="D111" t="n">
-        <v>153612.387550201</v>
+        <v>154165.903807615</v>
       </c>
       <c r="E111" t="n">
-        <v>153612.387550201</v>
+        <v>154165.903807615</v>
       </c>
       <c r="F111" t="n">
-        <v>76498969</v>
+        <v>76928786</v>
       </c>
     </row>
     <row r="112">
@@ -3412,13 +3412,13 @@
         <v>30.802498</v>
       </c>
       <c r="D112" t="n">
-        <v>102852.702811245</v>
+        <v>103178.627254509</v>
       </c>
       <c r="E112" t="n">
-        <v>102852.702811245</v>
+        <v>103178.627254509</v>
       </c>
       <c r="F112" t="n">
-        <v>51220646</v>
+        <v>51486135</v>
       </c>
     </row>
     <row r="113">
@@ -3432,13 +3432,13 @@
         <v>-88.8965</v>
       </c>
       <c r="D113" t="n">
-        <v>29947.3634538153</v>
+        <v>30035.9278557114</v>
       </c>
       <c r="E113" t="n">
-        <v>29947.3634538153</v>
+        <v>30035.9278557114</v>
       </c>
       <c r="F113" t="n">
-        <v>14913787</v>
+        <v>14987928</v>
       </c>
     </row>
     <row r="114">
@@ -3452,13 +3452,13 @@
         <v>10.2679</v>
       </c>
       <c r="D114" t="n">
-        <v>3923.66064257028</v>
+        <v>3932.97595190381</v>
       </c>
       <c r="E114" t="n">
-        <v>3923.66064257028</v>
+        <v>3932.97595190381</v>
       </c>
       <c r="F114" t="n">
-        <v>1953983</v>
+        <v>1962555</v>
       </c>
     </row>
     <row r="115">
@@ -3472,13 +3472,13 @@
         <v>39.7823</v>
       </c>
       <c r="D115" t="n">
-        <v>1083.0562248996</v>
+        <v>1089.19238476954</v>
       </c>
       <c r="E115" t="n">
-        <v>1083.0562248996</v>
+        <v>1089.19238476954</v>
       </c>
       <c r="F115" t="n">
-        <v>539362</v>
+        <v>543507</v>
       </c>
     </row>
     <row r="116">
@@ -3492,13 +3492,13 @@
         <v>25.0136</v>
       </c>
       <c r="D116" t="n">
-        <v>28821.6425702811</v>
+        <v>29024.2224448898</v>
       </c>
       <c r="E116" t="n">
-        <v>28821.6425702811</v>
+        <v>29024.2224448898</v>
       </c>
       <c r="F116" t="n">
-        <v>14353178</v>
+        <v>14483087</v>
       </c>
     </row>
     <row r="117">
@@ -3512,13 +3512,13 @@
         <v>31.4659</v>
       </c>
       <c r="D117" t="n">
-        <v>6979.27911646586</v>
+        <v>7002.61322645291</v>
       </c>
       <c r="E117" t="n">
-        <v>6979.27911646586</v>
+        <v>7002.61322645291</v>
       </c>
       <c r="F117" t="n">
-        <v>3475681</v>
+        <v>3494304</v>
       </c>
     </row>
     <row r="118">
@@ -3532,13 +3532,13 @@
         <v>40.4897</v>
       </c>
       <c r="D118" t="n">
-        <v>85290.7108433735</v>
+        <v>85665.4488977956</v>
       </c>
       <c r="E118" t="n">
-        <v>85290.7108433735</v>
+        <v>85665.4488977956</v>
       </c>
       <c r="F118" t="n">
-        <v>42474774</v>
+        <v>42747059</v>
       </c>
     </row>
     <row r="119">
@@ -3552,13 +3552,13 @@
         <v>178.065</v>
       </c>
       <c r="D119" t="n">
-        <v>45.2429718875502</v>
+        <v>46.2264529058116</v>
       </c>
       <c r="E119" t="n">
-        <v>45.2429718875502</v>
+        <v>46.2264529058116</v>
       </c>
       <c r="F119" t="n">
-        <v>22531</v>
+        <v>23067</v>
       </c>
     </row>
     <row r="120">
@@ -3572,13 +3572,13 @@
         <v>25.748151</v>
       </c>
       <c r="D120" t="n">
-        <v>27055.7610441767</v>
+        <v>27187.7394789579</v>
       </c>
       <c r="E120" t="n">
-        <v>27055.7610441767</v>
+        <v>27187.7394789579</v>
       </c>
       <c r="F120" t="n">
-        <v>13473769</v>
+        <v>13566682</v>
       </c>
     </row>
     <row r="121">
@@ -3592,13 +3592,13 @@
         <v>-53.1258</v>
       </c>
       <c r="D121" t="n">
-        <v>9065.63453815261</v>
+        <v>9096.29458917836</v>
       </c>
       <c r="E121" t="n">
-        <v>9065.63453815261</v>
+        <v>9096.29458917836</v>
       </c>
       <c r="F121" t="n">
-        <v>4514686</v>
+        <v>4539051</v>
       </c>
     </row>
     <row r="122">
@@ -3612,13 +3612,13 @@
         <v>149.4068</v>
       </c>
       <c r="D122" t="n">
-        <v>7700.65060240964</v>
+        <v>7723.0621242485</v>
       </c>
       <c r="E122" t="n">
-        <v>7700.65060240964</v>
+        <v>7723.0621242485</v>
       </c>
       <c r="F122" t="n">
-        <v>3834924</v>
+        <v>3853808</v>
       </c>
     </row>
     <row r="123">
@@ -3632,13 +3632,13 @@
         <v>-61.551</v>
       </c>
       <c r="D123" t="n">
-        <v>5249.22289156627</v>
+        <v>5272.51903807615</v>
       </c>
       <c r="E123" t="n">
-        <v>5249.22289156627</v>
+        <v>5272.51903807615</v>
       </c>
       <c r="F123" t="n">
-        <v>2614113</v>
+        <v>2630987</v>
       </c>
     </row>
     <row r="124">
@@ -3652,13 +3652,13 @@
         <v>-61.0242</v>
       </c>
       <c r="D124" t="n">
-        <v>3426.39959839357</v>
+        <v>3443.53907815631</v>
       </c>
       <c r="E124" t="n">
-        <v>3426.39959839357</v>
+        <v>3443.53907815631</v>
       </c>
       <c r="F124" t="n">
-        <v>1706347</v>
+        <v>1718326</v>
       </c>
     </row>
     <row r="125">
@@ -3672,13 +3672,13 @@
         <v>45.166244</v>
       </c>
       <c r="D125" t="n">
-        <v>6541.91767068273</v>
+        <v>6567.55110220441</v>
       </c>
       <c r="E125" t="n">
-        <v>6541.91767068273</v>
+        <v>6567.55110220441</v>
       </c>
       <c r="F125" t="n">
-        <v>3257875</v>
+        <v>3277208</v>
       </c>
     </row>
     <row r="126">
@@ -3692,13 +3692,13 @@
         <v>165.618042</v>
       </c>
       <c r="D126" t="n">
-        <v>40.8995983935743</v>
+        <v>41.0741482965932</v>
       </c>
       <c r="E126" t="n">
-        <v>40.8995983935743</v>
+        <v>41.0741482965932</v>
       </c>
       <c r="F126" t="n">
-        <v>20368</v>
+        <v>20496</v>
       </c>
     </row>
     <row r="127">
@@ -3712,13 +3712,13 @@
         <v>55.5364</v>
       </c>
       <c r="D127" t="n">
-        <v>6326.77309236948</v>
+        <v>6366.34869739479</v>
       </c>
       <c r="E127" t="n">
-        <v>6326.77309236948</v>
+        <v>6366.34869739479</v>
       </c>
       <c r="F127" t="n">
-        <v>3150733</v>
+        <v>3176808</v>
       </c>
     </row>
     <row r="128">
@@ -3732,13 +3732,13 @@
         <v>-62.8333</v>
       </c>
       <c r="D128" t="n">
-        <v>231.170682730924</v>
+        <v>232.721442885772</v>
       </c>
       <c r="E128" t="n">
-        <v>231.170682730924</v>
+        <v>232.721442885772</v>
       </c>
       <c r="F128" t="n">
-        <v>115123</v>
+        <v>116128</v>
       </c>
     </row>
     <row r="129">
@@ -3752,13 +3752,13 @@
         <v>-56.3159</v>
       </c>
       <c r="D129" t="n">
-        <v>11.218875502008</v>
+        <v>11.2464929859719</v>
       </c>
       <c r="E129" t="n">
-        <v>11.218875502008</v>
+        <v>11.2464929859719</v>
       </c>
       <c r="F129" t="n">
-        <v>5587</v>
+        <v>5612</v>
       </c>
     </row>
     <row r="130">
@@ -3772,13 +3772,13 @@
         <v>-63.0501</v>
       </c>
       <c r="D130" t="n">
-        <v>628.082329317269</v>
+        <v>630.911823647295</v>
       </c>
       <c r="E130" t="n">
-        <v>628.082329317269</v>
+        <v>630.911823647295</v>
       </c>
       <c r="F130" t="n">
-        <v>312785</v>
+        <v>314825</v>
       </c>
     </row>
     <row r="131">
@@ -3792,13 +3792,13 @@
         <v>-178.1165</v>
       </c>
       <c r="D131" t="n">
-        <v>68.8132530120482</v>
+        <v>69.5671342685371</v>
       </c>
       <c r="E131" t="n">
-        <v>68.8132530120482</v>
+        <v>69.5671342685371</v>
       </c>
       <c r="F131" t="n">
-        <v>34269</v>
+        <v>34714</v>
       </c>
     </row>
     <row r="132">
@@ -3812,13 +3812,13 @@
         <v>2.2137</v>
       </c>
       <c r="D132" t="n">
-        <v>1723686.27108434</v>
+        <v>1731523.6252505</v>
       </c>
       <c r="E132" t="n">
-        <v>1723686.27108434</v>
+        <v>1731523.6252505</v>
       </c>
       <c r="F132" t="n">
-        <v>858395763</v>
+        <v>864030289</v>
       </c>
     </row>
     <row r="133">
@@ -3832,13 +3832,13 @@
         <v>11.6094</v>
       </c>
       <c r="D133" t="n">
-        <v>8705.32730923695</v>
+        <v>8736.8376753507</v>
       </c>
       <c r="E133" t="n">
-        <v>8705.32730923695</v>
+        <v>8736.8376753507</v>
       </c>
       <c r="F133" t="n">
-        <v>4335253</v>
+        <v>4359682</v>
       </c>
     </row>
     <row r="134">
@@ -3852,13 +3852,13 @@
         <v>-15.3101</v>
       </c>
       <c r="D134" t="n">
-        <v>2559.54016064257</v>
+        <v>2566.4248496994</v>
       </c>
       <c r="E134" t="n">
-        <v>2559.54016064257</v>
+        <v>2566.4248496994</v>
       </c>
       <c r="F134" t="n">
-        <v>1274651</v>
+        <v>1280646</v>
       </c>
     </row>
     <row r="135">
@@ -3872,13 +3872,13 @@
         <v>43.3569</v>
       </c>
       <c r="D135" t="n">
-        <v>105547.502008032</v>
+        <v>106031.340681363</v>
       </c>
       <c r="E135" t="n">
-        <v>105547.502008032</v>
+        <v>106031.340681363</v>
       </c>
       <c r="F135" t="n">
-        <v>52562656</v>
+        <v>52909639</v>
       </c>
     </row>
     <row r="136">
@@ -3892,13 +3892,13 @@
         <v>10.451526</v>
       </c>
       <c r="D136" t="n">
-        <v>1082137.68473896</v>
+        <v>1087387.29258517</v>
       </c>
       <c r="E136" t="n">
-        <v>1082137.68473896</v>
+        <v>1087387.29258517</v>
       </c>
       <c r="F136" t="n">
-        <v>538904567</v>
+        <v>542606259</v>
       </c>
     </row>
     <row r="137">
@@ -3912,13 +3912,13 @@
         <v>-1.0232</v>
       </c>
       <c r="D137" t="n">
-        <v>42490.9277108434</v>
+        <v>42594.1743486974</v>
       </c>
       <c r="E137" t="n">
-        <v>42490.9277108434</v>
+        <v>42594.1743486974</v>
       </c>
       <c r="F137" t="n">
-        <v>21160482</v>
+        <v>21254493</v>
       </c>
     </row>
     <row r="138">
@@ -3932,13 +3932,13 @@
         <v>21.8243</v>
       </c>
       <c r="D138" t="n">
-        <v>92602.2690763052</v>
+        <v>93231.8256513026</v>
       </c>
       <c r="E138" t="n">
-        <v>92602.2690763052</v>
+        <v>93231.8256513026</v>
       </c>
       <c r="F138" t="n">
-        <v>46115930</v>
+        <v>46522681</v>
       </c>
     </row>
     <row r="139">
@@ -3952,13 +3952,13 @@
         <v>-61.679</v>
       </c>
       <c r="D139" t="n">
-        <v>63.0160642570281</v>
+        <v>63.2124248496994</v>
       </c>
       <c r="E139" t="n">
-        <v>63.0160642570281</v>
+        <v>63.2124248496994</v>
       </c>
       <c r="F139" t="n">
-        <v>31382</v>
+        <v>31543</v>
       </c>
     </row>
     <row r="140">
@@ -3972,13 +3972,13 @@
         <v>-90.2308</v>
       </c>
       <c r="D140" t="n">
-        <v>91960.5502008032</v>
+        <v>92294.5631262525</v>
       </c>
       <c r="E140" t="n">
-        <v>91960.5502008032</v>
+        <v>92294.5631262525</v>
       </c>
       <c r="F140" t="n">
-        <v>45796354</v>
+        <v>46054987</v>
       </c>
     </row>
     <row r="141">
@@ -3992,13 +3992,13 @@
         <v>-9.6966</v>
       </c>
       <c r="D141" t="n">
-        <v>9946.95983935743</v>
+        <v>9973.60921843687</v>
       </c>
       <c r="E141" t="n">
-        <v>9946.95983935743</v>
+        <v>9973.60921843687</v>
       </c>
       <c r="F141" t="n">
-        <v>4953586</v>
+        <v>4976831</v>
       </c>
     </row>
     <row r="142">
@@ -4012,13 +4012,13 @@
         <v>-15.1804</v>
       </c>
       <c r="D142" t="n">
-        <v>1985.50200803213</v>
+        <v>1989.10621242485</v>
       </c>
       <c r="E142" t="n">
-        <v>1985.50200803213</v>
+        <v>1989.10621242485</v>
       </c>
       <c r="F142" t="n">
-        <v>988780</v>
+        <v>992564</v>
       </c>
     </row>
     <row r="143">
@@ -4032,13 +4032,13 @@
         <v>-58.93018</v>
       </c>
       <c r="D143" t="n">
-        <v>4290.18875502008</v>
+        <v>4316.4128256513</v>
       </c>
       <c r="E143" t="n">
-        <v>4290.18875502008</v>
+        <v>4316.4128256513</v>
       </c>
       <c r="F143" t="n">
-        <v>2136514</v>
+        <v>2153890</v>
       </c>
     </row>
     <row r="144">
@@ -4052,13 +4052,13 @@
         <v>-72.2852</v>
       </c>
       <c r="D144" t="n">
-        <v>7210.19879518072</v>
+        <v>7225.67134268537</v>
       </c>
       <c r="E144" t="n">
-        <v>7210.19879518072</v>
+        <v>7225.67134268537</v>
       </c>
       <c r="F144" t="n">
-        <v>3590679</v>
+        <v>3605610</v>
       </c>
     </row>
     <row r="145">
@@ -4072,13 +4072,13 @@
         <v>12.4534</v>
       </c>
       <c r="D145" t="n">
-        <v>17.1887550200803</v>
+        <v>17.2084168336673</v>
       </c>
       <c r="E145" t="n">
-        <v>17.1887550200803</v>
+        <v>17.2084168336673</v>
       </c>
       <c r="F145" t="n">
-        <v>8560</v>
+        <v>8587</v>
       </c>
     </row>
     <row r="146">
@@ -4092,13 +4092,13 @@
         <v>-86.2419</v>
       </c>
       <c r="D146" t="n">
-        <v>84522.1465863454</v>
+        <v>84834.4909819639</v>
       </c>
       <c r="E146" t="n">
-        <v>84522.1465863454</v>
+        <v>84834.4909819639</v>
       </c>
       <c r="F146" t="n">
-        <v>42092029</v>
+        <v>42332411</v>
       </c>
     </row>
     <row r="147">
@@ -4112,13 +4112,13 @@
         <v>19.5033</v>
       </c>
       <c r="D147" t="n">
-        <v>205063.951807229</v>
+        <v>206266.833667335</v>
       </c>
       <c r="E147" t="n">
-        <v>205063.951807229</v>
+        <v>206266.833667335</v>
       </c>
       <c r="F147" t="n">
-        <v>102121848</v>
+        <v>102927150</v>
       </c>
     </row>
     <row r="148">
@@ -4132,13 +4132,13 @@
         <v>-19.0208</v>
       </c>
       <c r="D148" t="n">
-        <v>3523.09036144578</v>
+        <v>3529.16633266533</v>
       </c>
       <c r="E148" t="n">
-        <v>3523.09036144578</v>
+        <v>3529.16633266533</v>
       </c>
       <c r="F148" t="n">
-        <v>1754499</v>
+        <v>1761054</v>
       </c>
     </row>
     <row r="149">
@@ -4152,13 +4152,13 @@
         <v>78.96288</v>
       </c>
       <c r="D149" t="n">
-        <v>6706678.68674699</v>
+        <v>6750501.6753507</v>
       </c>
       <c r="E149" t="n">
-        <v>6706678.68674699</v>
+        <v>6750501.6753507</v>
       </c>
       <c r="F149" t="n">
-        <v>3339925986</v>
+        <v>3368500336</v>
       </c>
     </row>
     <row r="150">
@@ -4172,13 +4172,13 @@
         <v>113.9213</v>
       </c>
       <c r="D150" t="n">
-        <v>547152.799196787</v>
+        <v>549737.915831663</v>
       </c>
       <c r="E150" t="n">
-        <v>547152.799196787</v>
+        <v>549737.915831663</v>
       </c>
       <c r="F150" t="n">
-        <v>272482094</v>
+        <v>274319220</v>
       </c>
     </row>
     <row r="151">
@@ -4192,13 +4192,13 @@
         <v>53.688046</v>
       </c>
       <c r="D151" t="n">
-        <v>828482.477911647</v>
+        <v>832724.196392786</v>
       </c>
       <c r="E151" t="n">
-        <v>828482.477911647</v>
+        <v>832724.196392786</v>
       </c>
       <c r="F151" t="n">
-        <v>412584274</v>
+        <v>415529374</v>
       </c>
     </row>
     <row r="152">
@@ -4212,13 +4212,13 @@
         <v>43.679291</v>
       </c>
       <c r="D152" t="n">
-        <v>385792.578313253</v>
+        <v>387453.048096192</v>
       </c>
       <c r="E152" t="n">
-        <v>385792.578313253</v>
+        <v>387453.048096192</v>
       </c>
       <c r="F152" t="n">
-        <v>192124704</v>
+        <v>193339071</v>
       </c>
     </row>
     <row r="153">
@@ -4232,13 +4232,13 @@
         <v>-7.6921</v>
       </c>
       <c r="D153" t="n">
-        <v>88356.4678714859</v>
+        <v>88706.9599198397</v>
       </c>
       <c r="E153" t="n">
-        <v>88356.4678714859</v>
+        <v>88706.9599198397</v>
       </c>
       <c r="F153" t="n">
-        <v>44001521</v>
+        <v>44264773</v>
       </c>
     </row>
     <row r="154">
@@ -4252,13 +4252,13 @@
         <v>34.851612</v>
       </c>
       <c r="D154" t="n">
-        <v>314496.002008032</v>
+        <v>315548.178356713</v>
       </c>
       <c r="E154" t="n">
-        <v>314496.002008032</v>
+        <v>315548.178356713</v>
       </c>
       <c r="F154" t="n">
-        <v>156619009</v>
+        <v>157458541</v>
       </c>
     </row>
     <row r="155">
@@ -4272,13 +4272,13 @@
         <v>12.56738</v>
       </c>
       <c r="D155" t="n">
-        <v>1312398.16064257</v>
+        <v>1318235.36472946</v>
       </c>
       <c r="E155" t="n">
-        <v>1312398.16064257</v>
+        <v>1318235.36472946</v>
       </c>
       <c r="F155" t="n">
-        <v>653574284</v>
+        <v>657799447</v>
       </c>
     </row>
     <row r="156">
@@ -4292,13 +4292,13 @@
         <v>-77.2975</v>
       </c>
       <c r="D156" t="n">
-        <v>11986.0763052209</v>
+        <v>12059.5270541082</v>
       </c>
       <c r="E156" t="n">
-        <v>11986.0763052209</v>
+        <v>12059.5270541082</v>
       </c>
       <c r="F156" t="n">
-        <v>5969066</v>
+        <v>6017704</v>
       </c>
     </row>
     <row r="157">
@@ -4312,13 +4312,13 @@
         <v>138.252924</v>
       </c>
       <c r="D157" t="n">
-        <v>185515.578313253</v>
+        <v>186658.258517034</v>
       </c>
       <c r="E157" t="n">
-        <v>185515.578313253</v>
+        <v>186658.258517034</v>
       </c>
       <c r="F157" t="n">
-        <v>92386758</v>
+        <v>93142471</v>
       </c>
     </row>
     <row r="158">
@@ -4332,13 +4332,13 @@
         <v>36.51</v>
       </c>
       <c r="D158" t="n">
-        <v>187330.65060241</v>
+        <v>188435.240480962</v>
       </c>
       <c r="E158" t="n">
-        <v>187330.65060241</v>
+        <v>188435.240480962</v>
       </c>
       <c r="F158" t="n">
-        <v>93290664</v>
+        <v>94029185</v>
       </c>
     </row>
     <row r="159">
@@ -4352,13 +4352,13 @@
         <v>66.9237</v>
       </c>
       <c r="D159" t="n">
-        <v>144246.742971888</v>
+        <v>144854.014028056</v>
       </c>
       <c r="E159" t="n">
-        <v>144246.742971888</v>
+        <v>144854.014028056</v>
       </c>
       <c r="F159" t="n">
-        <v>71834878</v>
+        <v>72282153</v>
       </c>
     </row>
     <row r="160">
@@ -4372,13 +4372,13 @@
         <v>37.9062</v>
       </c>
       <c r="D160" t="n">
-        <v>57052.8915662651</v>
+        <v>57282.5611222445</v>
       </c>
       <c r="E160" t="n">
-        <v>57052.8915662651</v>
+        <v>57282.5611222445</v>
       </c>
       <c r="F160" t="n">
-        <v>28412340</v>
+        <v>28583998</v>
       </c>
     </row>
     <row r="161">
@@ -4392,13 +4392,13 @@
         <v>-168.734</v>
       </c>
       <c r="D161" t="n">
-        <v>0.0582329317269076</v>
+        <v>0.062124248496994</v>
       </c>
       <c r="E161" t="n">
-        <v>0.0582329317269076</v>
+        <v>0.062124248496994</v>
       </c>
       <c r="F161" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="162">
@@ -4412,13 +4412,13 @@
         <v>127.766922</v>
       </c>
       <c r="D162" t="n">
-        <v>42930.359437751</v>
+        <v>43130.6032064128</v>
       </c>
       <c r="E162" t="n">
-        <v>42930.359437751</v>
+        <v>43130.6032064128</v>
       </c>
       <c r="F162" t="n">
-        <v>21379319</v>
+        <v>21522171</v>
       </c>
     </row>
     <row r="163">
@@ -4432,13 +4432,13 @@
         <v>20.902977</v>
       </c>
       <c r="D163" t="n">
-        <v>32757.3032128514</v>
+        <v>32906.1883767535</v>
       </c>
       <c r="E163" t="n">
-        <v>32757.3032128514</v>
+        <v>32906.1883767535</v>
       </c>
       <c r="F163" t="n">
-        <v>16313137</v>
+        <v>16420188</v>
       </c>
     </row>
     <row r="164">
@@ -4452,13 +4452,13 @@
         <v>47.481766</v>
       </c>
       <c r="D164" t="n">
-        <v>109599.678714859</v>
+        <v>110007.873747495</v>
       </c>
       <c r="E164" t="n">
-        <v>109599.678714859</v>
+        <v>110007.873747495</v>
       </c>
       <c r="F164" t="n">
-        <v>54580640</v>
+        <v>54893929</v>
       </c>
     </row>
     <row r="165">
@@ -4472,13 +4472,13 @@
         <v>74.766098</v>
       </c>
       <c r="D165" t="n">
-        <v>46407.6204819277</v>
+        <v>46526.7234468938</v>
       </c>
       <c r="E165" t="n">
-        <v>46407.6204819277</v>
+        <v>46526.7234468938</v>
       </c>
       <c r="F165" t="n">
-        <v>23110995</v>
+        <v>23216835</v>
       </c>
     </row>
     <row r="166">
@@ -4492,13 +4492,13 @@
         <v>102.495496</v>
       </c>
       <c r="D166" t="n">
-        <v>133.64859437751</v>
+        <v>137.274549098196</v>
       </c>
       <c r="E166" t="n">
-        <v>133.64859437751</v>
+        <v>137.274549098196</v>
       </c>
       <c r="F166" t="n">
-        <v>66557</v>
+        <v>68500</v>
       </c>
     </row>
     <row r="167">
@@ -4512,13 +4512,13 @@
         <v>24.6032</v>
       </c>
       <c r="D167" t="n">
-        <v>31726.5281124498</v>
+        <v>31931.8096192385</v>
       </c>
       <c r="E167" t="n">
-        <v>31726.5281124498</v>
+        <v>31931.8096192385</v>
       </c>
       <c r="F167" t="n">
-        <v>15799811</v>
+        <v>15933973</v>
       </c>
     </row>
     <row r="168">
@@ -4532,13 +4532,13 @@
         <v>35.8623</v>
       </c>
       <c r="D168" t="n">
-        <v>148691.058232932</v>
+        <v>149477.266533066</v>
       </c>
       <c r="E168" t="n">
-        <v>148691.058232932</v>
+        <v>149477.266533066</v>
       </c>
       <c r="F168" t="n">
-        <v>74048147</v>
+        <v>74589156</v>
       </c>
     </row>
     <row r="169">
@@ -4552,13 +4552,13 @@
         <v>28.2336</v>
       </c>
       <c r="D169" t="n">
-        <v>3511.09437751004</v>
+        <v>3525.77354709419</v>
       </c>
       <c r="E169" t="n">
-        <v>3511.09437751004</v>
+        <v>3525.77354709419</v>
       </c>
       <c r="F169" t="n">
-        <v>1748525</v>
+        <v>1759361</v>
       </c>
     </row>
     <row r="170">
@@ -4572,13 +4572,13 @@
         <v>-9.429499</v>
       </c>
       <c r="D170" t="n">
-        <v>1175.03815261044</v>
+        <v>1177.13026052104</v>
       </c>
       <c r="E170" t="n">
-        <v>1175.03815261044</v>
+        <v>1177.13026052104</v>
       </c>
       <c r="F170" t="n">
-        <v>585169</v>
+        <v>587388</v>
       </c>
     </row>
     <row r="171">
@@ -4592,13 +4592,13 @@
         <v>17.228331</v>
       </c>
       <c r="D171" t="n">
-        <v>60645.4096385542</v>
+        <v>60897.7575150301</v>
       </c>
       <c r="E171" t="n">
-        <v>60645.4096385542</v>
+        <v>60897.7575150301</v>
       </c>
       <c r="F171" t="n">
-        <v>30201414</v>
+        <v>30387981</v>
       </c>
     </row>
     <row r="172">
@@ -4612,13 +4612,13 @@
         <v>9.55</v>
       </c>
       <c r="D172" t="n">
-        <v>1029.54618473896</v>
+        <v>1033.52905811623</v>
       </c>
       <c r="E172" t="n">
-        <v>1029.54618473896</v>
+        <v>1033.52905811623</v>
       </c>
       <c r="F172" t="n">
-        <v>512714</v>
+        <v>515731</v>
       </c>
     </row>
     <row r="173">
@@ -4632,13 +4632,13 @@
         <v>23.8813</v>
       </c>
       <c r="D173" t="n">
-        <v>75177.7690763052</v>
+        <v>75579.3066132265</v>
       </c>
       <c r="E173" t="n">
-        <v>75177.7690763052</v>
+        <v>75579.3066132265</v>
       </c>
       <c r="F173" t="n">
-        <v>37438529</v>
+        <v>37714074</v>
       </c>
     </row>
     <row r="174">
@@ -4652,13 +4652,13 @@
         <v>6.1296</v>
       </c>
       <c r="D174" t="n">
-        <v>24967.8614457831</v>
+        <v>25058.2825651303</v>
       </c>
       <c r="E174" t="n">
-        <v>24967.8614457831</v>
+        <v>25058.2825651303</v>
       </c>
       <c r="F174" t="n">
-        <v>12433995</v>
+        <v>12504083</v>
       </c>
     </row>
     <row r="175">
@@ -4672,13 +4672,13 @@
         <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>7.75100401606426</v>
+        <v>7.75350701402806</v>
       </c>
       <c r="E175" t="n">
-        <v>7.75100401606426</v>
+        <v>7.75350701402806</v>
       </c>
       <c r="F175" t="n">
-        <v>3860</v>
+        <v>3869</v>
       </c>
     </row>
     <row r="176">
@@ -4692,13 +4692,13 @@
         <v>46.869107</v>
       </c>
       <c r="D176" t="n">
-        <v>13543.5923694779</v>
+        <v>13599.5931863727</v>
       </c>
       <c r="E176" t="n">
-        <v>13543.5923694779</v>
+        <v>13599.5931863727</v>
       </c>
       <c r="F176" t="n">
-        <v>6744709</v>
+        <v>6786197</v>
       </c>
     </row>
     <row r="177">
@@ -4712,13 +4712,13 @@
         <v>34.3015</v>
       </c>
       <c r="D177" t="n">
-        <v>10788.2710843373</v>
+        <v>10835.5190380762</v>
       </c>
       <c r="E177" t="n">
-        <v>10788.2710843373</v>
+        <v>10835.5190380762</v>
       </c>
       <c r="F177" t="n">
-        <v>5372559</v>
+        <v>5406924</v>
       </c>
     </row>
     <row r="178">
@@ -4732,13 +4732,13 @@
         <v>101.975766</v>
       </c>
       <c r="D178" t="n">
-        <v>112151.463855422</v>
+        <v>113119.845691383</v>
       </c>
       <c r="E178" t="n">
-        <v>112151.463855422</v>
+        <v>113119.845691383</v>
       </c>
       <c r="F178" t="n">
-        <v>55851429</v>
+        <v>56446803</v>
       </c>
     </row>
     <row r="179">
@@ -4752,13 +4752,13 @@
         <v>73.2207</v>
       </c>
       <c r="D179" t="n">
-        <v>11569.1104417671</v>
+        <v>11679.2244488978</v>
       </c>
       <c r="E179" t="n">
-        <v>11569.1104417671</v>
+        <v>11679.2244488978</v>
       </c>
       <c r="F179" t="n">
-        <v>5761417</v>
+        <v>5827933</v>
       </c>
     </row>
     <row r="180">
@@ -4772,13 +4772,13 @@
         <v>-3.996166</v>
       </c>
       <c r="D180" t="n">
-        <v>4679.98795180723</v>
+        <v>4699.22845691383</v>
       </c>
       <c r="E180" t="n">
-        <v>4679.98795180723</v>
+        <v>4699.22845691383</v>
       </c>
       <c r="F180" t="n">
-        <v>2330634</v>
+        <v>2344915</v>
       </c>
     </row>
     <row r="181">
@@ -4792,13 +4792,13 @@
         <v>14.3754</v>
       </c>
       <c r="D181" t="n">
-        <v>9394.32530120482</v>
+        <v>9436.73547094188</v>
       </c>
       <c r="E181" t="n">
-        <v>9394.32530120482</v>
+        <v>9436.73547094188</v>
       </c>
       <c r="F181" t="n">
-        <v>4678374</v>
+        <v>4708931</v>
       </c>
     </row>
     <row r="182">
@@ -4812,13 +4812,13 @@
         <v>171.1845</v>
       </c>
       <c r="D182" t="n">
-        <v>1.64658634538153</v>
+        <v>1.65130260521042</v>
       </c>
       <c r="E182" t="n">
-        <v>1.64658634538153</v>
+        <v>1.65130260521042</v>
       </c>
       <c r="F182" t="n">
-        <v>820</v>
+        <v>824</v>
       </c>
     </row>
     <row r="183">
@@ -4832,13 +4832,13 @@
         <v>-10.9408</v>
       </c>
       <c r="D183" t="n">
-        <v>8399.91164658635</v>
+        <v>8422.54709418838</v>
       </c>
       <c r="E183" t="n">
-        <v>8399.91164658635</v>
+        <v>8422.54709418838</v>
       </c>
       <c r="F183" t="n">
-        <v>4183156</v>
+        <v>4202851</v>
       </c>
     </row>
     <row r="184">
@@ -4852,13 +4852,13 @@
         <v>57.552152</v>
       </c>
       <c r="D184" t="n">
-        <v>483.678714859438</v>
+        <v>485.557114228457</v>
       </c>
       <c r="E184" t="n">
-        <v>483.678714859438</v>
+        <v>485.557114228457</v>
       </c>
       <c r="F184" t="n">
-        <v>240872</v>
+        <v>242293</v>
       </c>
     </row>
     <row r="185">
@@ -4872,13 +4872,13 @@
         <v>-102.5528</v>
       </c>
       <c r="D185" t="n">
-        <v>944066.965863454</v>
+        <v>947038.418837675</v>
       </c>
       <c r="E185" t="n">
-        <v>944066.965863454</v>
+        <v>947038.418837675</v>
       </c>
       <c r="F185" t="n">
-        <v>470145349</v>
+        <v>472572171</v>
       </c>
     </row>
     <row r="186">
@@ -4892,13 +4892,13 @@
         <v>150.5508</v>
       </c>
       <c r="D186" t="n">
-        <v>0.267068273092369</v>
+        <v>0.268537074148297</v>
       </c>
       <c r="E186" t="n">
-        <v>0.267068273092369</v>
+        <v>0.268537074148297</v>
       </c>
       <c r="F186" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="187">
@@ -4912,13 +4912,13 @@
         <v>28.3699</v>
       </c>
       <c r="D187" t="n">
-        <v>88210.1606425703</v>
+        <v>88545.1182364729</v>
       </c>
       <c r="E187" t="n">
-        <v>88210.1606425703</v>
+        <v>88545.1182364729</v>
       </c>
       <c r="F187" t="n">
-        <v>43928660</v>
+        <v>44184014</v>
       </c>
     </row>
     <row r="188">
@@ -4932,13 +4932,13 @@
         <v>7.4167</v>
       </c>
       <c r="D188" t="n">
-        <v>751.979919678715</v>
+        <v>755.498997995992</v>
       </c>
       <c r="E188" t="n">
-        <v>751.979919678715</v>
+        <v>755.498997995992</v>
       </c>
       <c r="F188" t="n">
-        <v>374486</v>
+        <v>376994</v>
       </c>
     </row>
     <row r="189">
@@ -4952,13 +4952,13 @@
         <v>103.8467</v>
       </c>
       <c r="D189" t="n">
-        <v>5272.41164658635</v>
+        <v>5387.26653306613</v>
       </c>
       <c r="E189" t="n">
-        <v>5272.41164658635</v>
+        <v>5387.26653306613</v>
       </c>
       <c r="F189" t="n">
-        <v>2625661</v>
+        <v>2688246</v>
       </c>
     </row>
     <row r="190">
@@ -4972,13 +4972,13 @@
         <v>19.37439</v>
       </c>
       <c r="D190" t="n">
-        <v>30900.9096385542</v>
+        <v>31038.8176352705</v>
       </c>
       <c r="E190" t="n">
-        <v>30900.9096385542</v>
+        <v>31038.8176352705</v>
       </c>
       <c r="F190" t="n">
-        <v>15388653</v>
+        <v>15488370</v>
       </c>
     </row>
     <row r="191">
@@ -4992,13 +4992,13 @@
         <v>-7.0926</v>
       </c>
       <c r="D191" t="n">
-        <v>214126.700803213</v>
+        <v>214740.521042084</v>
       </c>
       <c r="E191" t="n">
-        <v>214126.700803213</v>
+        <v>214740.521042084</v>
       </c>
       <c r="F191" t="n">
-        <v>106635097</v>
+        <v>107155520</v>
       </c>
     </row>
     <row r="192">
@@ -5012,13 +5012,13 @@
         <v>35.529562</v>
       </c>
       <c r="D192" t="n">
-        <v>20607.124497992</v>
+        <v>20708.0420841683</v>
       </c>
       <c r="E192" t="n">
-        <v>20607.124497992</v>
+        <v>20708.0420841683</v>
       </c>
       <c r="F192" t="n">
-        <v>10262348</v>
+        <v>10333313</v>
       </c>
     </row>
     <row r="193">
@@ -5032,13 +5032,13 @@
         <v>18.4904</v>
       </c>
       <c r="D193" t="n">
-        <v>16336.140562249</v>
+        <v>16417.5931863727</v>
       </c>
       <c r="E193" t="n">
-        <v>16336.140562249</v>
+        <v>16417.5931863727</v>
       </c>
       <c r="F193" t="n">
-        <v>8135398</v>
+        <v>8192379</v>
       </c>
     </row>
     <row r="194">
@@ -5052,13 +5052,13 @@
         <v>84.25</v>
       </c>
       <c r="D194" t="n">
-        <v>139575.032128514</v>
+        <v>140451.507014028</v>
       </c>
       <c r="E194" t="n">
-        <v>139575.032128514</v>
+        <v>140451.507014028</v>
       </c>
       <c r="F194" t="n">
-        <v>69508366</v>
+        <v>70085302</v>
       </c>
     </row>
     <row r="195">
@@ -5072,13 +5072,13 @@
         <v>-69.9683</v>
       </c>
       <c r="D195" t="n">
-        <v>3825.75502008032</v>
+        <v>3840.16833667335</v>
       </c>
       <c r="E195" t="n">
-        <v>3825.75502008032</v>
+        <v>3840.16833667335</v>
       </c>
       <c r="F195" t="n">
-        <v>1905226</v>
+        <v>1916244</v>
       </c>
     </row>
     <row r="196">
@@ -5092,13 +5092,13 @@
         <v>-68.2385</v>
       </c>
       <c r="D196" t="n">
-        <v>192.592369477912</v>
+        <v>195.442885771543</v>
       </c>
       <c r="E196" t="n">
-        <v>192.592369477912</v>
+        <v>195.442885771543</v>
       </c>
       <c r="F196" t="n">
-        <v>95911</v>
+        <v>97526</v>
       </c>
     </row>
     <row r="197">
@@ -5112,13 +5112,13 @@
         <v>-68.99</v>
       </c>
       <c r="D197" t="n">
-        <v>2767.39959839357</v>
+        <v>2786.45490981964</v>
       </c>
       <c r="E197" t="n">
-        <v>2767.39959839357</v>
+        <v>2786.45490981964</v>
       </c>
       <c r="F197" t="n">
-        <v>1378165</v>
+        <v>1390441</v>
       </c>
     </row>
     <row r="198">
@@ -5132,13 +5132,13 @@
         <v>-63.0548</v>
       </c>
       <c r="D198" t="n">
-        <v>883.853413654619</v>
+        <v>886.987975951904</v>
       </c>
       <c r="E198" t="n">
-        <v>883.853413654619</v>
+        <v>886.987975951904</v>
       </c>
       <c r="F198" t="n">
-        <v>440159</v>
+        <v>442607</v>
       </c>
     </row>
     <row r="199">
@@ -5152,13 +5152,13 @@
         <v>5.2913</v>
       </c>
       <c r="D199" t="n">
-        <v>477612.819277108</v>
+        <v>479976.354709419</v>
       </c>
       <c r="E199" t="n">
-        <v>477612.819277108</v>
+        <v>479976.354709419</v>
       </c>
       <c r="F199" t="n">
-        <v>237851184</v>
+        <v>239508201</v>
       </c>
     </row>
     <row r="200">
@@ -5172,13 +5172,13 @@
         <v>174.886</v>
       </c>
       <c r="D200" t="n">
-        <v>1700.77510040161</v>
+        <v>1702.74148296593</v>
       </c>
       <c r="E200" t="n">
-        <v>1700.77510040161</v>
+        <v>1702.74148296593</v>
       </c>
       <c r="F200" t="n">
-        <v>846986</v>
+        <v>849668</v>
       </c>
     </row>
     <row r="201">
@@ -5192,13 +5192,13 @@
         <v>-85.207229</v>
       </c>
       <c r="D201" t="n">
-        <v>3934.32128514056</v>
+        <v>3941.42885771543</v>
       </c>
       <c r="E201" t="n">
-        <v>3934.32128514056</v>
+        <v>3941.42885771543</v>
       </c>
       <c r="F201" t="n">
-        <v>1959292</v>
+        <v>1966773</v>
       </c>
     </row>
     <row r="202">
@@ -5212,13 +5212,13 @@
         <v>8.081666</v>
       </c>
       <c r="D202" t="n">
-        <v>2145.95582329317</v>
+        <v>2152.50901803607</v>
       </c>
       <c r="E202" t="n">
-        <v>2145.95582329317</v>
+        <v>2152.50901803607</v>
       </c>
       <c r="F202" t="n">
-        <v>1068686</v>
+        <v>1074102</v>
       </c>
     </row>
     <row r="203">
@@ -5232,13 +5232,13 @@
         <v>8.6753</v>
       </c>
       <c r="D203" t="n">
-        <v>68421.4337349398</v>
+        <v>68618.3486973948</v>
       </c>
       <c r="E203" t="n">
-        <v>68421.4337349398</v>
+        <v>68618.3486973948</v>
       </c>
       <c r="F203" t="n">
-        <v>34073874</v>
+        <v>34240556</v>
       </c>
     </row>
     <row r="204">
@@ -5252,13 +5252,13 @@
         <v>21.7453</v>
       </c>
       <c r="D204" t="n">
-        <v>48737.4116465863</v>
+        <v>48951.0921843687</v>
       </c>
       <c r="E204" t="n">
-        <v>48737.4116465863</v>
+        <v>48951.0921843687</v>
       </c>
       <c r="F204" t="n">
-        <v>24271231</v>
+        <v>24426595</v>
       </c>
     </row>
     <row r="205">
@@ -5272,13 +5272,13 @@
         <v>8.4689</v>
       </c>
       <c r="D205" t="n">
-        <v>35712.7389558233</v>
+        <v>35894.1122244489</v>
       </c>
       <c r="E205" t="n">
-        <v>35712.7389558233</v>
+        <v>35894.1122244489</v>
       </c>
       <c r="F205" t="n">
-        <v>17784944</v>
+        <v>17911162</v>
       </c>
     </row>
     <row r="206">
@@ -5292,13 +5292,13 @@
         <v>55.923255</v>
       </c>
       <c r="D206" t="n">
-        <v>87755.5742971888</v>
+        <v>88022</v>
       </c>
       <c r="E206" t="n">
-        <v>87755.5742971888</v>
+        <v>88022</v>
       </c>
       <c r="F206" t="n">
-        <v>43702276</v>
+        <v>43922978</v>
       </c>
     </row>
     <row r="207">
@@ -5312,13 +5312,13 @@
         <v>69.3451</v>
       </c>
       <c r="D207" t="n">
-        <v>340113.226907631</v>
+        <v>341292.53507014</v>
       </c>
       <c r="E207" t="n">
-        <v>340113.226907631</v>
+        <v>341292.53507014</v>
       </c>
       <c r="F207" t="n">
-        <v>169376387</v>
+        <v>170304975</v>
       </c>
     </row>
     <row r="208">
@@ -5332,13 +5332,13 @@
         <v>-80.7821</v>
       </c>
       <c r="D208" t="n">
-        <v>150521.118473896</v>
+        <v>150981.410821643</v>
       </c>
       <c r="E208" t="n">
-        <v>150521.118473896</v>
+        <v>150981.410821643</v>
       </c>
       <c r="F208" t="n">
-        <v>74959517</v>
+        <v>75339724</v>
       </c>
     </row>
     <row r="209">
@@ -5352,13 +5352,13 @@
         <v>143.95555</v>
       </c>
       <c r="D209" t="n">
-        <v>1907.89759036145</v>
+        <v>1936.50901803607</v>
       </c>
       <c r="E209" t="n">
-        <v>1907.89759036145</v>
+        <v>1936.50901803607</v>
       </c>
       <c r="F209" t="n">
-        <v>950133</v>
+        <v>966318</v>
       </c>
     </row>
     <row r="210">
@@ -5372,13 +5372,13 @@
         <v>-58.4438</v>
       </c>
       <c r="D210" t="n">
-        <v>79625.6726907631</v>
+        <v>80196.9679358717</v>
       </c>
       <c r="E210" t="n">
-        <v>79625.6726907631</v>
+        <v>80196.9679358717</v>
       </c>
       <c r="F210" t="n">
-        <v>39653585</v>
+        <v>40018287</v>
       </c>
     </row>
     <row r="211">
@@ -5392,13 +5392,13 @@
         <v>-75.0152</v>
       </c>
       <c r="D211" t="n">
-        <v>740923.397590361</v>
+        <v>743377.322645291</v>
       </c>
       <c r="E211" t="n">
-        <v>740923.397590361</v>
+        <v>743377.322645291</v>
       </c>
       <c r="F211" t="n">
-        <v>368979852</v>
+        <v>370945284</v>
       </c>
     </row>
     <row r="212">
@@ -5412,13 +5412,13 @@
         <v>121.774017</v>
       </c>
       <c r="D212" t="n">
-        <v>340061.403614458</v>
+        <v>341880.71743487</v>
       </c>
       <c r="E212" t="n">
-        <v>340061.403614458</v>
+        <v>341880.71743487</v>
       </c>
       <c r="F212" t="n">
-        <v>169350579</v>
+        <v>170598478</v>
       </c>
     </row>
     <row r="213">
@@ -5432,13 +5432,13 @@
         <v>19.1451</v>
       </c>
       <c r="D213" t="n">
-        <v>787492.899598394</v>
+        <v>791674.460921844</v>
       </c>
       <c r="E213" t="n">
-        <v>787492.899598394</v>
+        <v>791674.460921844</v>
       </c>
       <c r="F213" t="n">
-        <v>392171464</v>
+        <v>395045556</v>
       </c>
     </row>
     <row r="214">
@@ -5452,13 +5452,13 @@
         <v>-8.2245</v>
       </c>
       <c r="D214" t="n">
-        <v>291887.917670683</v>
+        <v>293008.44488978</v>
       </c>
       <c r="E214" t="n">
-        <v>291887.917670683</v>
+        <v>293008.44488978</v>
       </c>
       <c r="F214" t="n">
-        <v>145360183</v>
+        <v>146211214</v>
       </c>
     </row>
     <row r="215">
@@ -5472,13 +5472,13 @@
         <v>51.1839</v>
       </c>
       <c r="D215" t="n">
-        <v>107754.712851406</v>
+        <v>107975.805611222</v>
       </c>
       <c r="E215" t="n">
-        <v>107754.712851406</v>
+        <v>107975.805611222</v>
       </c>
       <c r="F215" t="n">
-        <v>53661847</v>
+        <v>53879927</v>
       </c>
     </row>
     <row r="216">
@@ -5492,13 +5492,13 @@
         <v>24.9668</v>
       </c>
       <c r="D216" t="n">
-        <v>356213.331325301</v>
+        <v>357660.4749499</v>
       </c>
       <c r="E216" t="n">
-        <v>356213.331325301</v>
+        <v>357660.4749499</v>
       </c>
       <c r="F216" t="n">
-        <v>177394239</v>
+        <v>178472577</v>
       </c>
     </row>
     <row r="217">
@@ -5512,13 +5512,13 @@
         <v>105.318756</v>
       </c>
       <c r="D217" t="n">
-        <v>1908879.53012048</v>
+        <v>1915155.10220441</v>
       </c>
       <c r="E217" t="n">
-        <v>1908879.53012048</v>
+        <v>1915155.10220441</v>
       </c>
       <c r="F217" t="n">
-        <v>950622006</v>
+        <v>955662396</v>
       </c>
     </row>
     <row r="218">
@@ -5532,13 +5532,13 @@
         <v>29.8739</v>
       </c>
       <c r="D218" t="n">
-        <v>7787.24497991968</v>
+        <v>7825.98597194389</v>
       </c>
       <c r="E218" t="n">
-        <v>7787.24497991968</v>
+        <v>7825.98597194389</v>
       </c>
       <c r="F218" t="n">
-        <v>3878048</v>
+        <v>3905167</v>
       </c>
     </row>
     <row r="219">
@@ -5552,13 +5552,13 @@
         <v>-62.782998</v>
       </c>
       <c r="D219" t="n">
-        <v>23.078313253012</v>
+        <v>23.1823647294589</v>
       </c>
       <c r="E219" t="n">
-        <v>23.078313253012</v>
+        <v>23.1823647294589</v>
       </c>
       <c r="F219" t="n">
-        <v>11493</v>
+        <v>11568</v>
       </c>
     </row>
     <row r="220">
@@ -5572,13 +5572,13 @@
         <v>-60.9789</v>
       </c>
       <c r="D220" t="n">
-        <v>1050.71686746988</v>
+        <v>1058.83567134269</v>
       </c>
       <c r="E220" t="n">
-        <v>1050.71686746988</v>
+        <v>1058.83567134269</v>
       </c>
       <c r="F220" t="n">
-        <v>523257</v>
+        <v>528359</v>
       </c>
     </row>
     <row r="221">
@@ -5592,13 +5592,13 @@
         <v>-61.2872</v>
       </c>
       <c r="D221" t="n">
-        <v>477.24297188755</v>
+        <v>480.382765531062</v>
       </c>
       <c r="E221" t="n">
-        <v>477.24297188755</v>
+        <v>480.382765531062</v>
       </c>
       <c r="F221" t="n">
-        <v>237667</v>
+        <v>239711</v>
       </c>
     </row>
     <row r="222">
@@ -5612,13 +5612,13 @@
         <v>-172.1046</v>
       </c>
       <c r="D222" t="n">
-        <v>0.98995983935743</v>
+        <v>0.993987975951904</v>
       </c>
       <c r="E222" t="n">
-        <v>0.98995983935743</v>
+        <v>0.993987975951904</v>
       </c>
       <c r="F222" t="n">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="223">
@@ -5632,13 +5632,13 @@
         <v>12.4578</v>
       </c>
       <c r="D223" t="n">
-        <v>1751.53614457831</v>
+        <v>1758.22645290581</v>
       </c>
       <c r="E223" t="n">
-        <v>1751.53614457831</v>
+        <v>1758.22645290581</v>
       </c>
       <c r="F223" t="n">
-        <v>872265</v>
+        <v>877355</v>
       </c>
     </row>
     <row r="224">
@@ -5652,13 +5652,13 @@
         <v>6.6131</v>
       </c>
       <c r="D224" t="n">
-        <v>964.449799196787</v>
+        <v>967.224448897796</v>
       </c>
       <c r="E224" t="n">
-        <v>964.449799196787</v>
+        <v>967.224448897796</v>
       </c>
       <c r="F224" t="n">
-        <v>480296</v>
+        <v>482645</v>
       </c>
     </row>
     <row r="225">
@@ -5672,13 +5672,13 @@
         <v>45.079162</v>
       </c>
       <c r="D225" t="n">
-        <v>250834.212851406</v>
+        <v>251241.793587174</v>
       </c>
       <c r="E225" t="n">
-        <v>250834.212851406</v>
+        <v>251241.793587174</v>
       </c>
       <c r="F225" t="n">
-        <v>124915438</v>
+        <v>125369655</v>
       </c>
     </row>
     <row r="226">
@@ -5692,13 +5692,13 @@
         <v>-14.4524</v>
       </c>
       <c r="D226" t="n">
-        <v>16183.2068273092</v>
+        <v>16234.0200400802</v>
       </c>
       <c r="E226" t="n">
-        <v>16183.2068273092</v>
+        <v>16234.0200400802</v>
       </c>
       <c r="F226" t="n">
-        <v>8059237</v>
+        <v>8100776</v>
       </c>
     </row>
     <row r="227">
@@ -5712,13 +5712,13 @@
         <v>21.0059</v>
       </c>
       <c r="D227" t="n">
-        <v>197761.53815261</v>
+        <v>198794.49498998</v>
       </c>
       <c r="E227" t="n">
-        <v>197761.53815261</v>
+        <v>198794.49498998</v>
       </c>
       <c r="F227" t="n">
-        <v>98485246</v>
+        <v>99198453</v>
       </c>
     </row>
     <row r="228">
@@ -5732,13 +5732,13 @@
         <v>55.492</v>
       </c>
       <c r="D228" t="n">
-        <v>1313.66265060241</v>
+        <v>1334.31863727455</v>
       </c>
       <c r="E228" t="n">
-        <v>1313.66265060241</v>
+        <v>1334.31863727455</v>
       </c>
       <c r="F228" t="n">
-        <v>654204</v>
+        <v>665825</v>
       </c>
     </row>
     <row r="229">
@@ -5752,13 +5752,13 @@
         <v>-11.779889</v>
       </c>
       <c r="D229" t="n">
-        <v>2058.12851405622</v>
+        <v>2062.34468937876</v>
       </c>
       <c r="E229" t="n">
-        <v>2058.12851405622</v>
+        <v>2062.34468937876</v>
       </c>
       <c r="F229" t="n">
-        <v>1024948</v>
+        <v>1029110</v>
       </c>
     </row>
     <row r="230">
@@ -5772,13 +5772,13 @@
         <v>103.8333</v>
       </c>
       <c r="D230" t="n">
-        <v>43624.1104417671</v>
+        <v>43661.2264529058</v>
       </c>
       <c r="E230" t="n">
-        <v>43624.1104417671</v>
+        <v>43661.2264529058</v>
       </c>
       <c r="F230" t="n">
-        <v>21724807</v>
+        <v>21786952</v>
       </c>
     </row>
     <row r="231">
@@ -5792,13 +5792,13 @@
         <v>19.699</v>
       </c>
       <c r="D231" t="n">
-        <v>115158.911646586</v>
+        <v>115709.953907816</v>
       </c>
       <c r="E231" t="n">
-        <v>115158.911646586</v>
+        <v>115709.953907816</v>
       </c>
       <c r="F231" t="n">
-        <v>57349138</v>
+        <v>57739267</v>
       </c>
     </row>
     <row r="232">
@@ -5812,13 +5812,13 @@
         <v>14.9955</v>
       </c>
       <c r="D232" t="n">
-        <v>73402.5702811245</v>
+        <v>73765.875751503</v>
       </c>
       <c r="E232" t="n">
-        <v>73402.5702811245</v>
+        <v>73765.875751503</v>
       </c>
       <c r="F232" t="n">
-        <v>36554480</v>
+        <v>36809172</v>
       </c>
     </row>
     <row r="233">
@@ -5832,13 +5832,13 @@
         <v>160.1562</v>
       </c>
       <c r="D233" t="n">
-        <v>7.82730923694779</v>
+        <v>7.85170340681363</v>
       </c>
       <c r="E233" t="n">
-        <v>7.82730923694779</v>
+        <v>7.85170340681363</v>
       </c>
       <c r="F233" t="n">
-        <v>3898</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="234">
@@ -5852,13 +5852,13 @@
         <v>46.199616</v>
       </c>
       <c r="D234" t="n">
-        <v>4559.17670682731</v>
+        <v>4579.49699398798</v>
       </c>
       <c r="E234" t="n">
-        <v>4559.17670682731</v>
+        <v>4579.49699398798</v>
       </c>
       <c r="F234" t="n">
-        <v>2270470</v>
+        <v>2285169</v>
       </c>
     </row>
     <row r="235">
@@ -5872,13 +5872,13 @@
         <v>22.9375</v>
       </c>
       <c r="D235" t="n">
-        <v>708038.530120482</v>
+        <v>709964.76753507</v>
       </c>
       <c r="E235" t="n">
-        <v>708038.530120482</v>
+        <v>709964.76753507</v>
       </c>
       <c r="F235" t="n">
-        <v>352603188</v>
+        <v>354272419</v>
       </c>
     </row>
     <row r="236">
@@ -5892,13 +5892,13 @@
         <v>31.307</v>
       </c>
       <c r="D236" t="n">
-        <v>3597.09236947791</v>
+        <v>3611.30260521042</v>
       </c>
       <c r="E236" t="n">
-        <v>3597.09236947791</v>
+        <v>3611.30260521042</v>
       </c>
       <c r="F236" t="n">
-        <v>1791352</v>
+        <v>1802040</v>
       </c>
     </row>
     <row r="237">
@@ -5912,13 +5912,13 @@
         <v>-3.74922</v>
       </c>
       <c r="D237" t="n">
-        <v>1332755.78313253</v>
+        <v>1337485.75551102</v>
       </c>
       <c r="E237" t="n">
-        <v>1332755.78313253</v>
+        <v>1337485.75551102</v>
       </c>
       <c r="F237" t="n">
-        <v>663712380</v>
+        <v>667405392</v>
       </c>
     </row>
     <row r="238">
@@ -5932,13 +5932,13 @@
         <v>80.771797</v>
       </c>
       <c r="D238" t="n">
-        <v>32987.1706827309</v>
+        <v>33313.5370741483</v>
       </c>
       <c r="E238" t="n">
-        <v>32987.1706827309</v>
+        <v>33313.5370741483</v>
       </c>
       <c r="F238" t="n">
-        <v>16427611</v>
+        <v>16623455</v>
       </c>
     </row>
     <row r="239">
@@ -5952,13 +5952,13 @@
         <v>30.2176</v>
       </c>
       <c r="D239" t="n">
-        <v>15611.0200803213</v>
+        <v>15651.1903807615</v>
       </c>
       <c r="E239" t="n">
-        <v>15611.0200803213</v>
+        <v>15651.1903807615</v>
       </c>
       <c r="F239" t="n">
-        <v>7774288</v>
+        <v>7809944</v>
       </c>
     </row>
     <row r="240">
@@ -5972,13 +5972,13 @@
         <v>-56.0278</v>
       </c>
       <c r="D240" t="n">
-        <v>4436.0843373494</v>
+        <v>4458.60921843687</v>
       </c>
       <c r="E240" t="n">
-        <v>4436.0843373494</v>
+        <v>4458.60921843687</v>
       </c>
       <c r="F240" t="n">
-        <v>2209170</v>
+        <v>2224846</v>
       </c>
     </row>
     <row r="241">
@@ -5992,13 +5992,13 @@
         <v>18.643501</v>
       </c>
       <c r="D241" t="n">
-        <v>294058.050200803</v>
+        <v>295627.058116232</v>
       </c>
       <c r="E241" t="n">
-        <v>294058.050200803</v>
+        <v>295627.058116232</v>
       </c>
       <c r="F241" t="n">
-        <v>146440909</v>
+        <v>147517902</v>
       </c>
     </row>
     <row r="242">
@@ -6012,13 +6012,13 @@
         <v>8.2275</v>
       </c>
       <c r="D242" t="n">
-        <v>238317.815261044</v>
+        <v>239236.619238477</v>
       </c>
       <c r="E242" t="n">
-        <v>238317.815261044</v>
+        <v>239236.619238477</v>
       </c>
       <c r="F242" t="n">
-        <v>118682272</v>
+        <v>119379073</v>
       </c>
     </row>
     <row r="243">
@@ -6032,13 +6032,13 @@
         <v>38.996815</v>
       </c>
       <c r="D243" t="n">
-        <v>7214.53815261044</v>
+        <v>7249.36072144289</v>
       </c>
       <c r="E243" t="n">
-        <v>7214.53815261044</v>
+        <v>7249.36072144289</v>
       </c>
       <c r="F243" t="n">
-        <v>3592840</v>
+        <v>3617431</v>
       </c>
     </row>
     <row r="244">
@@ -6052,13 +6052,13 @@
         <v>121</v>
       </c>
       <c r="D244" t="n">
-        <v>752.652610441767</v>
+        <v>771.132264529058</v>
       </c>
       <c r="E244" t="n">
-        <v>752.652610441767</v>
+        <v>771.132264529058</v>
       </c>
       <c r="F244" t="n">
-        <v>374821</v>
+        <v>384795</v>
       </c>
     </row>
     <row r="245">
@@ -6072,13 +6072,13 @@
         <v>71.2761</v>
       </c>
       <c r="D245" t="n">
-        <v>8115.40963855422</v>
+        <v>8125.81563126253</v>
       </c>
       <c r="E245" t="n">
-        <v>8115.40963855422</v>
+        <v>8125.81563126253</v>
       </c>
       <c r="F245" t="n">
-        <v>4041474</v>
+        <v>4054782</v>
       </c>
     </row>
     <row r="246">
@@ -6092,13 +6092,13 @@
         <v>34.888822</v>
       </c>
       <c r="D246" t="n">
-        <v>415.897590361446</v>
+        <v>416.084168336673</v>
       </c>
       <c r="E246" t="n">
-        <v>415.897590361446</v>
+        <v>416.084168336673</v>
       </c>
       <c r="F246" t="n">
-        <v>207117</v>
+        <v>207626</v>
       </c>
     </row>
     <row r="247">
@@ -6112,13 +6112,13 @@
         <v>100.992541</v>
       </c>
       <c r="D247" t="n">
-        <v>15628.3654618474</v>
+        <v>15936.4208416834</v>
       </c>
       <c r="E247" t="n">
-        <v>15628.3654618474</v>
+        <v>15936.4208416834</v>
       </c>
       <c r="F247" t="n">
-        <v>7782926</v>
+        <v>7952274</v>
       </c>
     </row>
     <row r="248">
@@ -6132,13 +6132,13 @@
         <v>125.727539</v>
       </c>
       <c r="D248" t="n">
-        <v>426.020080321285</v>
+        <v>440.040080160321</v>
       </c>
       <c r="E248" t="n">
-        <v>426.020080321285</v>
+        <v>440.040080160321</v>
       </c>
       <c r="F248" t="n">
-        <v>212158</v>
+        <v>219580</v>
       </c>
     </row>
     <row r="249">
@@ -6152,13 +6152,13 @@
         <v>0.8248</v>
       </c>
       <c r="D249" t="n">
-        <v>3504.58232931727</v>
+        <v>3524.63927855711</v>
       </c>
       <c r="E249" t="n">
-        <v>3504.58232931727</v>
+        <v>3524.63927855711</v>
       </c>
       <c r="F249" t="n">
-        <v>1745282</v>
+        <v>1758795</v>
       </c>
     </row>
     <row r="250">
@@ -6172,13 +6172,13 @@
         <v>-61.2225</v>
       </c>
       <c r="D250" t="n">
-        <v>4450.71887550201</v>
+        <v>4492.44488977956</v>
       </c>
       <c r="E250" t="n">
-        <v>4450.71887550201</v>
+        <v>4492.44488977956</v>
       </c>
       <c r="F250" t="n">
-        <v>2216458</v>
+        <v>2241730</v>
       </c>
     </row>
     <row r="251">
@@ -6192,13 +6192,13 @@
         <v>9.537499</v>
       </c>
       <c r="D251" t="n">
-        <v>92701.4638554217</v>
+        <v>93218.0681362725</v>
       </c>
       <c r="E251" t="n">
-        <v>92701.4638554217</v>
+        <v>93218.0681362725</v>
       </c>
       <c r="F251" t="n">
-        <v>46165329</v>
+        <v>46515816</v>
       </c>
     </row>
     <row r="252">
@@ -6212,13 +6212,13 @@
         <v>35.2433</v>
       </c>
       <c r="D252" t="n">
-        <v>1285047.15662651</v>
+        <v>1293033.63326653</v>
       </c>
       <c r="E252" t="n">
-        <v>1285047.15662651</v>
+        <v>1293033.63326653</v>
       </c>
       <c r="F252" t="n">
-        <v>639953484</v>
+        <v>645223783</v>
       </c>
     </row>
     <row r="253">
@@ -6232,13 +6232,13 @@
         <v>-100</v>
       </c>
       <c r="D253" t="n">
-        <v>12412289.4638554</v>
+        <v>12454201.4168337</v>
       </c>
       <c r="E253" t="n">
-        <v>12412289.4638554</v>
+        <v>12454201.4168337</v>
       </c>
       <c r="F253" t="n">
-        <v>6181320153</v>
+        <v>6214646507</v>
       </c>
     </row>
     <row r="254">
@@ -6252,13 +6252,13 @@
         <v>32.290275</v>
       </c>
       <c r="D254" t="n">
-        <v>16479.1445783133</v>
+        <v>16545.8376753507</v>
       </c>
       <c r="E254" t="n">
-        <v>16479.1445783133</v>
+        <v>16545.8376753507</v>
       </c>
       <c r="F254" t="n">
-        <v>8206614</v>
+        <v>8256373</v>
       </c>
     </row>
     <row r="255">
@@ -6272,13 +6272,13 @@
         <v>31.1656</v>
       </c>
       <c r="D255" t="n">
-        <v>642488.881526104</v>
+        <v>645746.837675351</v>
       </c>
       <c r="E255" t="n">
-        <v>642488.881526104</v>
+        <v>645746.837675351</v>
       </c>
       <c r="F255" t="n">
-        <v>319959463</v>
+        <v>322227672</v>
       </c>
     </row>
     <row r="256">
@@ -6292,13 +6292,13 @@
         <v>53.847818</v>
       </c>
       <c r="D256" t="n">
-        <v>172744.831325301</v>
+        <v>173554.855711423</v>
       </c>
       <c r="E256" t="n">
-        <v>172744.831325301</v>
+        <v>173554.855711423</v>
       </c>
       <c r="F256" t="n">
-        <v>86026926</v>
+        <v>86603873</v>
       </c>
     </row>
     <row r="257">
@@ -6312,13 +6312,13 @@
         <v>-63.0686</v>
       </c>
       <c r="D257" t="n">
-        <v>14.6084337349398</v>
+        <v>14.7975951903808</v>
       </c>
       <c r="E257" t="n">
-        <v>14.6084337349398</v>
+        <v>14.7975951903808</v>
       </c>
       <c r="F257" t="n">
-        <v>7275</v>
+        <v>7384</v>
       </c>
     </row>
     <row r="258">
@@ -6332,13 +6332,13 @@
         <v>-64.7505</v>
       </c>
       <c r="D258" t="n">
-        <v>515.497991967871</v>
+        <v>519.462925851703</v>
       </c>
       <c r="E258" t="n">
-        <v>515.497991967871</v>
+        <v>519.462925851703</v>
       </c>
       <c r="F258" t="n">
-        <v>256718</v>
+        <v>259212</v>
       </c>
     </row>
     <row r="259">
@@ -6352,13 +6352,13 @@
         <v>-64.64</v>
       </c>
       <c r="D259" t="n">
-        <v>69.6787148594377</v>
+        <v>70.0360721442886</v>
       </c>
       <c r="E259" t="n">
-        <v>69.6787148594377</v>
+        <v>70.0360721442886</v>
       </c>
       <c r="F259" t="n">
-        <v>34700</v>
+        <v>34948</v>
       </c>
     </row>
     <row r="260">
@@ -6372,13 +6372,13 @@
         <v>-81.2546</v>
       </c>
       <c r="D260" t="n">
-        <v>252.052208835341</v>
+        <v>252.717434869739</v>
       </c>
       <c r="E260" t="n">
-        <v>252.052208835341</v>
+        <v>252.717434869739</v>
       </c>
       <c r="F260" t="n">
-        <v>125522</v>
+        <v>126106</v>
       </c>
     </row>
     <row r="261">
@@ -6392,13 +6392,13 @@
         <v>-2.3644</v>
       </c>
       <c r="D261" t="n">
-        <v>1655.50803212851</v>
+        <v>1660.33867735471</v>
       </c>
       <c r="E261" t="n">
-        <v>1655.50803212851</v>
+        <v>1660.33867735471</v>
       </c>
       <c r="F261" t="n">
-        <v>824443</v>
+        <v>828509</v>
       </c>
     </row>
     <row r="262">
@@ -6412,13 +6412,13 @@
         <v>-59.5236</v>
       </c>
       <c r="D262" t="n">
-        <v>23.6325301204819</v>
+        <v>23.7114228456914</v>
       </c>
       <c r="E262" t="n">
-        <v>23.6325301204819</v>
+        <v>23.7114228456914</v>
       </c>
       <c r="F262" t="n">
-        <v>11769</v>
+        <v>11832</v>
       </c>
     </row>
     <row r="263">
@@ -6432,13 +6432,13 @@
         <v>-5.3536</v>
       </c>
       <c r="D263" t="n">
-        <v>1499.75903614458</v>
+        <v>1505.36873747495</v>
       </c>
       <c r="E263" t="n">
-        <v>1499.75903614458</v>
+        <v>1505.36873747495</v>
       </c>
       <c r="F263" t="n">
-        <v>746880</v>
+        <v>751179</v>
       </c>
     </row>
     <row r="264">
@@ -6452,13 +6452,13 @@
         <v>-4.5481</v>
       </c>
       <c r="D264" t="n">
-        <v>510.21686746988</v>
+        <v>512.390781563126</v>
       </c>
       <c r="E264" t="n">
-        <v>510.21686746988</v>
+        <v>512.390781563126</v>
       </c>
       <c r="F264" t="n">
-        <v>254088</v>
+        <v>255683</v>
       </c>
     </row>
     <row r="265">
@@ -6472,13 +6472,13 @@
         <v>-62.187366</v>
       </c>
       <c r="D265" t="n">
-        <v>12.3212851405622</v>
+        <v>12.3366733466934</v>
       </c>
       <c r="E265" t="n">
-        <v>12.3212851405622</v>
+        <v>12.3366733466934</v>
       </c>
       <c r="F265" t="n">
-        <v>6136</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="266">
@@ -6492,13 +6492,13 @@
         <v>-14.3559</v>
       </c>
       <c r="D266" t="n">
-        <v>1.81124497991968</v>
+        <v>1.81563126252505</v>
       </c>
       <c r="E266" t="n">
-        <v>1.81124497991968</v>
+        <v>1.81563126252505</v>
       </c>
       <c r="F266" t="n">
-        <v>902</v>
+        <v>906</v>
       </c>
     </row>
     <row r="267">
@@ -6512,13 +6512,13 @@
         <v>-71.7979</v>
       </c>
       <c r="D267" t="n">
-        <v>814.835341365462</v>
+        <v>818.048096192385</v>
       </c>
       <c r="E267" t="n">
-        <v>814.835341365462</v>
+        <v>818.048096192385</v>
       </c>
       <c r="F267" t="n">
-        <v>405788</v>
+        <v>408206</v>
       </c>
     </row>
     <row r="268">
@@ -6532,13 +6532,13 @@
         <v>-3.436</v>
       </c>
       <c r="D268" t="n">
-        <v>1603421.84738956</v>
+        <v>1609226.36873748</v>
       </c>
       <c r="E268" t="n">
-        <v>1603421.84738956</v>
+        <v>1609226.36873748</v>
       </c>
       <c r="F268" t="n">
-        <v>798504080</v>
+        <v>803003958</v>
       </c>
     </row>
     <row r="269">
@@ -6552,13 +6552,13 @@
         <v>-55.7658</v>
       </c>
       <c r="D269" t="n">
-        <v>36743.062248996</v>
+        <v>37279.4709418838</v>
       </c>
       <c r="E269" t="n">
-        <v>36743.062248996</v>
+        <v>37279.4709418838</v>
       </c>
       <c r="F269" t="n">
-        <v>18298045</v>
+        <v>18602456</v>
       </c>
     </row>
     <row r="270">
@@ -6572,13 +6572,13 @@
         <v>64.585262</v>
       </c>
       <c r="D270" t="n">
-        <v>45400.1024096386</v>
+        <v>45511.5190380761</v>
       </c>
       <c r="E270" t="n">
-        <v>45400.1024096386</v>
+        <v>45511.5190380761</v>
       </c>
       <c r="F270" t="n">
-        <v>22609251</v>
+        <v>22710248</v>
       </c>
     </row>
     <row r="271">
@@ -6592,13 +6592,13 @@
         <v>166.9592</v>
       </c>
       <c r="D271" t="n">
-        <v>0.847389558232932</v>
+        <v>0.853707414829659</v>
       </c>
       <c r="E271" t="n">
-        <v>0.847389558232932</v>
+        <v>0.853707414829659</v>
       </c>
       <c r="F271" t="n">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="272">
@@ -6612,13 +6612,13 @@
         <v>-66.5897</v>
       </c>
       <c r="D272" t="n">
-        <v>74091.078313253</v>
+        <v>74419.5791583166</v>
       </c>
       <c r="E272" t="n">
-        <v>74091.078313253</v>
+        <v>74419.5791583166</v>
       </c>
       <c r="F272" t="n">
-        <v>36897357</v>
+        <v>37135370</v>
       </c>
     </row>
     <row r="273">
@@ -6632,13 +6632,13 @@
         <v>108.277199</v>
       </c>
       <c r="D273" t="n">
-        <v>1297.22489959839</v>
+        <v>1310.78356713427</v>
       </c>
       <c r="E273" t="n">
-        <v>1297.22489959839</v>
+        <v>1310.78356713427</v>
       </c>
       <c r="F273" t="n">
-        <v>646018</v>
+        <v>654081</v>
       </c>
     </row>
     <row r="274">
@@ -6652,13 +6652,13 @@
         <v>35.2332</v>
       </c>
       <c r="D274" t="n">
-        <v>86452.0180722892</v>
+        <v>86898.6733466934</v>
       </c>
       <c r="E274" t="n">
-        <v>86452.0180722892</v>
+        <v>86898.6733466934</v>
       </c>
       <c r="F274" t="n">
-        <v>43053105</v>
+        <v>43362438</v>
       </c>
     </row>
     <row r="275">
@@ -6672,13 +6672,13 @@
         <v>48.516388</v>
       </c>
       <c r="D275" t="n">
-        <v>1986.05421686747</v>
+        <v>1995.63527054108</v>
       </c>
       <c r="E275" t="n">
-        <v>1986.05421686747</v>
+        <v>1995.63527054108</v>
       </c>
       <c r="F275" t="n">
-        <v>989055</v>
+        <v>995822</v>
       </c>
     </row>
     <row r="276">
@@ -6692,13 +6692,13 @@
         <v>27.849332</v>
       </c>
       <c r="D276" t="n">
-        <v>27864.7590361446</v>
+        <v>28004.0841683367</v>
       </c>
       <c r="E276" t="n">
-        <v>27864.7590361446</v>
+        <v>28004.0841683367</v>
       </c>
       <c r="F276" t="n">
-        <v>13876650</v>
+        <v>13974038</v>
       </c>
     </row>
     <row r="277">
@@ -6712,13 +6712,13 @@
         <v>29.154857</v>
       </c>
       <c r="D277" t="n">
-        <v>13334.3674698795</v>
+        <v>13385.9859719439</v>
       </c>
       <c r="E277" t="n">
-        <v>13334.3674698795</v>
+        <v>13385.9859719439</v>
       </c>
       <c r="F277" t="n">
-        <v>6640515</v>
+        <v>6679607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>